<commit_message>
[queue 2개, deque 활용] 문제 해결
Signed-off-by: sjshi <sjshi@DESKTOP-TI47F0L>
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjshi\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="9980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="238">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1422,31 +1422,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:L184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="G69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="3.625" customWidth="1"/>
-    <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="1" max="2" width="3.58203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.58203125" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.875" customWidth="1"/>
-    <col min="11" max="11" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.83203125" customWidth="1"/>
+    <col min="11" max="11" width="47.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.45">
       <c r="I3" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>175</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -1681,7 +1681,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -1697,7 +1697,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -1734,7 +1734,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E18" s="2"/>
       <c r="H18" t="s">
         <v>28</v>
@@ -1746,7 +1746,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" ht="68.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D20" s="5" t="s">
         <v>205</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -1881,7 +1881,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D29" s="5" t="s">
         <v>202</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="4:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="68" x14ac:dyDescent="0.45">
       <c r="D30" s="8"/>
       <c r="E30" s="9" t="s">
         <v>207</v>
@@ -1994,7 +1994,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="4:12" ht="132" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" ht="136" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>51</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="50.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:12" ht="34.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>204</v>
       </c>
@@ -2125,7 +2125,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E39" s="1" t="s">
         <v>61</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E40" s="2"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -2193,7 +2193,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>64</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E43" s="2"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -2233,7 +2233,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E45" s="1" t="s">
         <v>69</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E46" s="2"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -2273,7 +2273,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>74</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E49" s="2"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -2313,7 +2313,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E50" s="1" t="s">
         <v>77</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E51" s="2"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -2338,7 +2338,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>80</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E53" s="2"/>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -2363,7 +2363,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E55" s="2"/>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -2388,7 +2388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E56" s="1" t="s">
         <v>86</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E57" s="1"/>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -2413,7 +2413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D58" s="5" t="s">
         <v>89</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>92</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E60" t="s">
         <v>226</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.45">
       <c r="H61" t="s">
         <v>95</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>100</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E65" t="s">
         <v>103</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>106</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="4:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:11" ht="68" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="4:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="4:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>112</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="4:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>114</v>
       </c>
@@ -2676,6 +2676,9 @@
       <c r="H71" t="s">
         <v>115</v>
       </c>
+      <c r="I71" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="J71" t="s">
         <v>236</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
         <v>117</v>
       </c>
@@ -2694,11 +2697,14 @@
       <c r="H72" t="s">
         <v>116</v>
       </c>
+      <c r="I72" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="J72" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
@@ -2712,16 +2718,22 @@
       <c r="H73" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="74" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="I73" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
         <v>121</v>
       </c>
       <c r="H74" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="75" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="I74" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E75" s="1" t="s">
         <v>122</v>
       </c>
@@ -2736,7 +2748,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E76" s="1" t="s">
         <v>124</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:11" x14ac:dyDescent="0.45">
       <c r="D78" t="s">
         <v>126</v>
       </c>
@@ -2769,7 +2781,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E79" t="s">
         <v>130</v>
       </c>
@@ -2781,7 +2793,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="80" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:11" x14ac:dyDescent="0.45">
       <c r="E80" s="1" t="s">
         <v>131</v>
       </c>
@@ -2796,7 +2808,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E81" s="1" t="s">
         <v>133</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E82" s="1" t="s">
         <v>135</v>
       </c>
@@ -2826,7 +2838,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E83" s="1" t="s">
         <v>137</v>
       </c>
@@ -2841,7 +2853,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E84" s="1" t="s">
         <v>139</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E85" s="1" t="s">
         <v>141</v>
       </c>
@@ -2871,7 +2883,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E86" s="1" t="s">
         <v>143</v>
       </c>
@@ -2886,7 +2898,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E87" s="1" t="s">
         <v>145</v>
       </c>
@@ -2901,7 +2913,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E88" s="1" t="s">
         <v>147</v>
       </c>
@@ -2916,7 +2928,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E89" s="1" t="s">
         <v>149</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E90" s="1" t="s">
         <v>151</v>
       </c>
@@ -2946,7 +2958,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E91" s="1" t="s">
         <v>153</v>
       </c>
@@ -2961,7 +2973,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E92" s="1" t="s">
         <v>156</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E93" s="1" t="s">
         <v>157</v>
       </c>
@@ -2991,7 +3003,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E94" s="1" t="s">
         <v>159</v>
       </c>
@@ -3006,7 +3018,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E95" s="1" t="s">
         <v>161</v>
       </c>
@@ -3021,12 +3033,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:8" x14ac:dyDescent="0.45">
       <c r="H96" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E97" s="1" t="s">
         <v>164</v>
       </c>
@@ -3041,7 +3053,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E98" s="1" t="s">
         <v>166</v>
       </c>
@@ -3056,7 +3068,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E99" s="1" t="s">
         <v>168</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E100" s="1" t="s">
         <v>170</v>
       </c>
@@ -3086,7 +3098,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E101" s="1" t="s">
         <v>172</v>
       </c>
@@ -3101,35 +3113,35 @@
         <v>173</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H102" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J103" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E181" t="str">
         <f>IF(D181="","",CONCATENATE("https://www.acmicpc.net/problem/",D181))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E182" t="str">
         <f>IF(D182="","",CONCATENATE("https://www.acmicpc.net/problem/",D182))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E183" t="str">
         <f>IF(D183="","",CONCATENATE("https://www.acmicpc.net/problem/",D183))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E184" t="str">
         <f>IF(D184="","",CONCATENATE("https://www.acmicpc.net/problem/",D184))</f>
         <v/>

</xml_diff>

<commit_message>
[graph complete & add dp template java file]
Signed-off-by: admin <admin@DESKTOP-0K8LBFF>
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjshi\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="9980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="242">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1009,12 +1009,52 @@
 클립보드 수마다 답이 여러 개가 있을 수 있다면 2차원 배열로 관리해라 ex)d[s][c]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>check 배열을 따로 관리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>해야 한다.c[n][m][2]
+안그러면 정답이 달라진다.
+대부분은 같은데 예외케이스가 존재한다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원래 했던 소스 뭐때문에 틀렸는지 모르겠다.
+Queue를 처음부터 끝까지 일관성 있게 돌리지 않으면 에러가 발생하는 가능성이 생기는것 같은데.. 왜 발생하는지 이유를 모르겠다.--&gt; 오답나오는 테스트케이스가 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다 똑같은데 if("D") chk[ny][nx]=chk[y][x]+1 이런식으로 마무리했다가 오류남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤경우에 달라지는지 예외케이스를 파악하지 못함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1048,6 +1088,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1100,7 +1148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1139,6 +1187,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1422,31 +1476,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:L184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="C65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.58203125" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.58203125" customWidth="1"/>
-    <col min="6" max="6" width="12.08203125" customWidth="1"/>
+    <col min="1" max="2" width="3.625" customWidth="1"/>
+    <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.625" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.83203125" customWidth="1"/>
-    <col min="11" max="11" width="47.58203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.25" customWidth="1"/>
+    <col min="11" max="11" width="47.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I3" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1478,7 +1532,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>175</v>
       </c>
@@ -1502,7 +1556,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1520,7 +1574,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1538,7 +1592,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1559,7 +1613,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1634,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1601,7 +1655,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1619,7 +1673,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1647,7 +1701,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1665,7 +1719,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -1681,7 +1735,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -1697,7 +1751,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1772,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -1734,7 +1788,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>
       <c r="H18" t="s">
         <v>28</v>
@@ -1746,7 +1800,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1764,7 +1818,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="68.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:12" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D20" s="5" t="s">
         <v>205</v>
       </c>
@@ -1790,7 +1844,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +1862,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1826,7 +1880,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
@@ -1844,7 +1898,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1865,7 +1919,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -1881,7 +1935,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1902,7 +1956,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -1923,7 +1977,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1944,7 +1998,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5" t="s">
         <v>202</v>
       </c>
@@ -1970,7 +2024,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="4:12" ht="68" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:12" ht="66" x14ac:dyDescent="0.3">
       <c r="D30" s="8"/>
       <c r="E30" s="9" t="s">
         <v>207</v>
@@ -1994,7 +2048,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="4:12" ht="136" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:12" ht="132" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2018,7 +2072,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2039,7 +2093,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="E33" s="1" t="s">
         <v>51</v>
       </c>
@@ -2060,7 +2114,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
@@ -2078,7 +2132,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -2099,7 +2153,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="34.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:12" ht="50.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D36" s="5" t="s">
         <v>204</v>
       </c>
@@ -2125,7 +2179,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -2146,7 +2200,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
@@ -2168,7 +2222,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E39" s="1" t="s">
         <v>61</v>
       </c>
@@ -2183,7 +2237,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E40" s="2"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -2193,7 +2247,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
@@ -2208,7 +2262,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E42" s="1" t="s">
         <v>64</v>
       </c>
@@ -2223,7 +2277,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E43" s="2"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -2233,7 +2287,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
@@ -2248,7 +2302,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="s">
         <v>69</v>
       </c>
@@ -2263,7 +2317,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E46" s="2"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -2273,7 +2327,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
@@ -2288,7 +2342,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E48" s="1" t="s">
         <v>74</v>
       </c>
@@ -2303,7 +2357,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E49" s="2"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -2313,7 +2367,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E50" s="1" t="s">
         <v>77</v>
       </c>
@@ -2328,7 +2382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E51" s="2"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -2338,7 +2392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E52" s="1" t="s">
         <v>80</v>
       </c>
@@ -2353,7 +2407,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E53" s="2"/>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -2363,7 +2417,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
@@ -2378,7 +2432,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E55" s="2"/>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -2388,7 +2442,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E56" s="1" t="s">
         <v>86</v>
       </c>
@@ -2403,7 +2457,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -2413,7 +2467,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D58" s="5" t="s">
         <v>89</v>
       </c>
@@ -2439,7 +2493,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="4:12" ht="51" x14ac:dyDescent="0.45">
+    <row r="59" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="E59" s="1" t="s">
         <v>92</v>
       </c>
@@ -2463,7 +2517,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="4:12" ht="51" x14ac:dyDescent="0.45">
+    <row r="60" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>226</v>
       </c>
@@ -2477,7 +2531,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
       <c r="H61" t="s">
         <v>95</v>
       </c>
@@ -2488,7 +2542,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
@@ -2509,7 +2563,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="34" x14ac:dyDescent="0.45">
+    <row r="63" spans="4:12" ht="33" x14ac:dyDescent="0.3">
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
@@ -2530,7 +2584,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E64" s="1" t="s">
         <v>100</v>
       </c>
@@ -2548,7 +2602,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>103</v>
       </c>
@@ -2563,7 +2617,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E66" s="1" t="s">
         <v>104</v>
       </c>
@@ -2581,7 +2635,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E67" s="1" t="s">
         <v>106</v>
       </c>
@@ -2599,7 +2653,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="4:11" ht="68" x14ac:dyDescent="0.45">
+    <row r="68" spans="4:11" ht="66" x14ac:dyDescent="0.3">
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -2620,7 +2674,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="4:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="69" spans="4:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
@@ -2641,7 +2695,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="4:11" ht="85" x14ac:dyDescent="0.45">
+    <row r="70" spans="4:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="E70" s="1" t="s">
         <v>112</v>
       </c>
@@ -2662,7 +2716,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="4:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="71" spans="4:11" ht="33" x14ac:dyDescent="0.3">
       <c r="E71" s="1" t="s">
         <v>114</v>
       </c>
@@ -2686,7 +2740,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="72" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
         <v>117</v>
       </c>
@@ -2704,7 +2758,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
@@ -2722,7 +2776,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E74" t="s">
         <v>121</v>
       </c>
@@ -2733,7 +2787,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="4:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="E75" s="1" t="s">
         <v>122</v>
       </c>
@@ -2747,8 +2801,14 @@
       <c r="H75" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="J75" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="K75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="E76" s="1" t="s">
         <v>124</v>
       </c>
@@ -2762,8 +2822,14 @@
       <c r="H76" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="78" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="J76" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D78" t="s">
         <v>126</v>
       </c>
@@ -2781,7 +2847,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E79" t="s">
         <v>130</v>
       </c>
@@ -2793,7 +2859,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="80" spans="4:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E80" s="1" t="s">
         <v>131</v>
       </c>
@@ -2808,7 +2874,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E81" s="1" t="s">
         <v>133</v>
       </c>
@@ -2823,7 +2889,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E82" s="1" t="s">
         <v>135</v>
       </c>
@@ -2838,7 +2904,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E83" s="1" t="s">
         <v>137</v>
       </c>
@@ -2853,7 +2919,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E84" s="1" t="s">
         <v>139</v>
       </c>
@@ -2868,7 +2934,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E85" s="1" t="s">
         <v>141</v>
       </c>
@@ -2883,7 +2949,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E86" s="1" t="s">
         <v>143</v>
       </c>
@@ -2898,7 +2964,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E87" s="1" t="s">
         <v>145</v>
       </c>
@@ -2913,7 +2979,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E88" s="1" t="s">
         <v>147</v>
       </c>
@@ -2928,7 +2994,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E89" s="1" t="s">
         <v>149</v>
       </c>
@@ -2943,7 +3009,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E90" s="1" t="s">
         <v>151</v>
       </c>
@@ -2958,7 +3024,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E91" s="1" t="s">
         <v>153</v>
       </c>
@@ -2973,7 +3039,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E92" s="1" t="s">
         <v>156</v>
       </c>
@@ -2988,7 +3054,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E93" s="1" t="s">
         <v>157</v>
       </c>
@@ -3003,7 +3069,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E94" s="1" t="s">
         <v>159</v>
       </c>
@@ -3018,7 +3084,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E95" s="1" t="s">
         <v>161</v>
       </c>
@@ -3033,12 +3099,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="5:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="5:8" x14ac:dyDescent="0.3">
       <c r="H96" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E97" s="1" t="s">
         <v>164</v>
       </c>
@@ -3053,7 +3119,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E98" s="1" t="s">
         <v>166</v>
       </c>
@@ -3068,7 +3134,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E99" s="1" t="s">
         <v>168</v>
       </c>
@@ -3083,7 +3149,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E100" s="1" t="s">
         <v>170</v>
       </c>
@@ -3098,7 +3164,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E101" s="1" t="s">
         <v>172</v>
       </c>
@@ -3113,35 +3179,35 @@
         <v>173</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
       <c r="H102" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J103" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.45">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E181" t="str">
         <f>IF(D181="","",CONCATENATE("https://www.acmicpc.net/problem/",D181))</f>
         <v/>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.45">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E182" t="str">
         <f>IF(D182="","",CONCATENATE("https://www.acmicpc.net/problem/",D182))</f>
         <v/>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.45">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E183" t="str">
         <f>IF(D183="","",CONCATENATE("https://www.acmicpc.net/problem/",D183))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.45">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E184" t="str">
         <f>IF(D184="","",CONCATENATE("https://www.acmicpc.net/problem/",D184))</f>
         <v/>

</xml_diff>

<commit_message>
add(l43236) : solution 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjshi\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="9980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="575">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3232,6 +3232,14 @@
   </si>
   <si>
     <t>3차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>못품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3830,27 +3838,27 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="3.625" customWidth="1"/>
-    <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="1" max="2" width="3.58203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.58203125" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.25" customWidth="1"/>
-    <col min="11" max="11" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.45">
       <c r="I3" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -3882,7 +3890,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>172</v>
       </c>
@@ -3906,7 +3914,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3924,7 +3932,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -3942,7 +3950,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3963,7 +3971,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
@@ -3984,7 +3992,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -4005,7 +4013,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
@@ -4023,7 +4031,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -4051,7 +4059,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
@@ -4069,7 +4077,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -4085,7 +4093,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -4101,7 +4109,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4122,7 +4130,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -4138,7 +4146,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E18" s="2"/>
       <c r="H18" t="s">
         <v>28</v>
@@ -4150,7 +4158,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
@@ -4168,7 +4176,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" ht="68.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D20" s="5" t="s">
         <v>202</v>
       </c>
@@ -4194,7 +4202,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4212,7 +4220,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
@@ -4230,7 +4238,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
@@ -4248,7 +4256,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4269,7 +4277,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -4285,7 +4293,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
@@ -4306,7 +4314,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -4327,7 +4335,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4348,7 +4356,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D29" s="5" t="s">
         <v>199</v>
       </c>
@@ -4374,7 +4382,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="4:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="68" x14ac:dyDescent="0.45">
       <c r="D30" s="8"/>
       <c r="E30" s="9" t="s">
         <v>204</v>
@@ -4398,7 +4406,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="4:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" ht="119" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -4422,7 +4430,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -4443,7 +4451,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>51</v>
       </c>
@@ -4464,7 +4472,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
@@ -4482,7 +4490,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -4503,7 +4511,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:12" ht="34.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>201</v>
       </c>
@@ -4529,7 +4537,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -4550,7 +4558,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
@@ -4572,7 +4580,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E39" s="1" t="s">
         <v>61</v>
       </c>
@@ -4587,7 +4595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E40" s="2"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -4597,7 +4605,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
@@ -4612,7 +4620,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>64</v>
       </c>
@@ -4627,7 +4635,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E43" s="2"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -4637,7 +4645,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
@@ -4652,7 +4660,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E45" s="1" t="s">
         <v>69</v>
       </c>
@@ -4667,7 +4675,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E46" s="2"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -4677,7 +4685,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
@@ -4692,7 +4700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>74</v>
       </c>
@@ -4707,7 +4715,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E49" s="2"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -4717,7 +4725,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E50" s="1" t="s">
         <v>77</v>
       </c>
@@ -4732,7 +4740,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E51" s="2"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -4742,7 +4750,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>80</v>
       </c>
@@ -4757,7 +4765,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E53" s="2"/>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -4767,7 +4775,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
@@ -4782,7 +4790,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E55" s="2"/>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -4792,7 +4800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E56" s="1" t="s">
         <v>86</v>
       </c>
@@ -4807,7 +4815,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E57" s="1"/>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -4817,7 +4825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D58" s="5" t="s">
         <v>89</v>
       </c>
@@ -4843,7 +4851,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>92</v>
       </c>
@@ -4867,7 +4875,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E60" t="s">
         <v>221</v>
       </c>
@@ -4881,7 +4889,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.45">
       <c r="H61" t="s">
         <v>95</v>
       </c>
@@ -4892,7 +4900,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
@@ -4913,7 +4921,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
@@ -4934,7 +4942,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>100</v>
       </c>
@@ -4952,7 +4960,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E65" t="s">
         <v>103</v>
       </c>
@@ -4967,7 +4975,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>104</v>
       </c>
@@ -4985,7 +4993,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>106</v>
       </c>
@@ -5003,7 +5011,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -5024,7 +5032,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
@@ -5045,7 +5053,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>112</v>
       </c>
@@ -5066,7 +5074,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>114</v>
       </c>
@@ -5090,7 +5098,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
         <v>117</v>
       </c>
@@ -5108,7 +5116,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
@@ -5126,7 +5134,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
         <v>121</v>
       </c>
@@ -5137,7 +5145,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E75" s="1" t="s">
         <v>122</v>
       </c>
@@ -5161,7 +5169,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="76" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E76" s="1" t="s">
         <v>124</v>
       </c>
@@ -5185,25 +5193,25 @@
         <v>235</v>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E183" t="str">
         <f>IF(D183="","",CONCATENATE("https://www.acmicpc.net/problem/",D183))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E184" t="str">
         <f>IF(D184="","",CONCATENATE("https://www.acmicpc.net/problem/",D184))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E185" t="str">
         <f>IF(D185="","",CONCATENATE("https://www.acmicpc.net/problem/",D185))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E186" t="str">
         <f>IF(D186="","",CONCATENATE("https://www.acmicpc.net/problem/",D186))</f>
         <v/>
@@ -5224,22 +5232,22 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="22.75" customWidth="1"/>
-    <col min="5" max="5" width="26.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08203125" customWidth="1"/>
     <col min="7" max="7" width="37.5" customWidth="1"/>
     <col min="8" max="8" width="62" customWidth="1"/>
     <col min="9" max="9" width="9.75" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="62.875" customWidth="1"/>
-    <col min="12" max="12" width="34.875" customWidth="1"/>
+    <col min="11" max="11" width="62.83203125" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" customWidth="1"/>
     <col min="13" max="13" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.45">
       <c r="J2" s="1" t="s">
         <v>278</v>
       </c>
@@ -5247,7 +5255,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -5282,7 +5290,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>249</v>
       </c>
@@ -5290,7 +5298,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="99" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="102" x14ac:dyDescent="0.45">
       <c r="E5" s="14" t="s">
         <v>257</v>
       </c>
@@ -5317,7 +5325,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" ht="51" x14ac:dyDescent="0.45">
       <c r="E6" s="14" t="s">
         <v>258</v>
       </c>
@@ -5334,7 +5342,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>128</v>
       </c>
@@ -5358,7 +5366,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>130</v>
       </c>
@@ -5382,7 +5390,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>132</v>
       </c>
@@ -5403,7 +5411,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>134</v>
       </c>
@@ -5424,7 +5432,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>136</v>
       </c>
@@ -5445,7 +5453,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
@@ -5466,7 +5474,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>140</v>
       </c>
@@ -5487,7 +5495,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>142</v>
       </c>
@@ -5508,7 +5516,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E15" s="1" t="s">
         <v>144</v>
       </c>
@@ -5529,7 +5537,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>146</v>
       </c>
@@ -5553,7 +5561,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E17" s="1" t="s">
         <v>148</v>
       </c>
@@ -5574,7 +5582,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
@@ -5598,7 +5606,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E19" s="1" t="s">
         <v>153</v>
       </c>
@@ -5622,7 +5630,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="20" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E20" s="1" t="s">
         <v>154</v>
       </c>
@@ -5646,7 +5654,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>156</v>
       </c>
@@ -5667,7 +5675,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>158</v>
       </c>
@@ -5688,7 +5696,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="23" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="H23" t="s">
         <v>160</v>
       </c>
@@ -5702,7 +5710,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:11" ht="68" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
@@ -5726,7 +5734,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="H25" t="s">
         <v>162</v>
       </c>
@@ -5740,7 +5748,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>163</v>
       </c>
@@ -5761,7 +5769,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>165</v>
       </c>
@@ -5785,7 +5793,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E28" s="1" t="s">
         <v>167</v>
       </c>
@@ -5806,7 +5814,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E29" s="1" t="s">
         <v>169</v>
       </c>
@@ -5830,7 +5838,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H30" t="s">
         <v>171</v>
       </c>
@@ -5841,7 +5849,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>245</v>
       </c>
@@ -5865,7 +5873,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H32" t="s">
         <v>246</v>
       </c>
@@ -5876,7 +5884,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>243</v>
       </c>
@@ -5900,7 +5908,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>240</v>
       </c>
@@ -5921,7 +5929,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="35" spans="4:13" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:13" ht="51.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>239</v>
       </c>
@@ -5945,7 +5953,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>250</v>
       </c>
@@ -5959,7 +5967,7 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E37" s="15" t="s">
         <v>251</v>
       </c>
@@ -5977,7 +5985,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H38" t="s">
         <v>253</v>
       </c>
@@ -5985,7 +5993,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H39" t="s">
         <v>254</v>
       </c>
@@ -5993,7 +6001,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H40" t="s">
         <v>255</v>
       </c>
@@ -6001,7 +6009,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H41" t="s">
         <v>290</v>
       </c>
@@ -6009,7 +6017,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>292</v>
       </c>
@@ -6027,7 +6035,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H43" t="s">
         <v>294</v>
       </c>
@@ -6035,7 +6043,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E44" s="14" t="s">
         <v>309</v>
       </c>
@@ -6053,7 +6061,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="45" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E45" s="14" t="s">
         <v>307</v>
       </c>
@@ -6064,7 +6072,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E46" s="1" t="s">
         <v>300</v>
       </c>
@@ -6082,7 +6090,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>301</v>
       </c>
@@ -6100,7 +6108,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>303</v>
       </c>
@@ -6118,7 +6126,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="49" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E49" s="14" t="s">
         <v>308</v>
       </c>
@@ -6136,7 +6144,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="50" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E50" s="14" t="s">
         <v>310</v>
       </c>
@@ -6147,7 +6155,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E51" s="1" t="s">
         <v>312</v>
       </c>
@@ -6165,7 +6173,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>314</v>
       </c>
@@ -6183,7 +6191,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E53" s="1" t="s">
         <v>316</v>
       </c>
@@ -6201,7 +6209,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>318</v>
       </c>
@@ -6219,7 +6227,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E55" s="1" t="s">
         <v>320</v>
       </c>
@@ -6237,7 +6245,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H56" t="s">
         <v>322</v>
       </c>
@@ -6245,7 +6253,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E57" s="1" t="s">
         <v>323</v>
       </c>
@@ -6263,7 +6271,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E58" s="1" t="s">
         <v>326</v>
       </c>
@@ -6281,7 +6289,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>327</v>
       </c>
@@ -6299,7 +6307,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E60" s="1" t="s">
         <v>329</v>
       </c>
@@ -6317,7 +6325,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="61" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E61" s="1" t="s">
         <v>331</v>
       </c>
@@ -6335,7 +6343,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="62" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D62" s="5" t="s">
         <v>333</v>
       </c>
@@ -6349,7 +6357,7 @@
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
     </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>243</v>
       </c>
@@ -6367,7 +6375,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>335</v>
       </c>
@@ -6385,7 +6393,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E65" s="1" t="s">
         <v>337</v>
       </c>
@@ -6403,7 +6411,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>339</v>
       </c>
@@ -6421,7 +6429,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>142</v>
       </c>
@@ -6436,7 +6444,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>341</v>
       </c>
@@ -6454,7 +6462,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>343</v>
       </c>
@@ -6472,7 +6480,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>345</v>
       </c>
@@ -6490,7 +6498,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>347</v>
       </c>
@@ -6508,7 +6516,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E72" s="1" t="s">
         <v>349</v>
       </c>
@@ -6526,7 +6534,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H73" t="s">
         <v>355</v>
       </c>
@@ -6534,7 +6542,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H74" t="s">
         <v>356</v>
       </c>
@@ -6542,7 +6550,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H75" t="s">
         <v>357</v>
       </c>
@@ -6550,7 +6558,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="H76" t="s">
         <v>358</v>
       </c>
@@ -6558,7 +6566,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D77" s="5" t="s">
         <v>359</v>
       </c>
@@ -6572,7 +6580,7 @@
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E78" s="1" t="s">
         <v>361</v>
       </c>
@@ -6590,7 +6598,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E79" s="1" t="s">
         <v>363</v>
       </c>
@@ -6608,7 +6616,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E80" s="1" t="s">
         <v>365</v>
       </c>
@@ -6626,7 +6634,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G81" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -6638,7 +6646,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E82" s="1" t="s">
         <v>366</v>
       </c>
@@ -6651,7 +6659,7 @@
       </c>
       <c r="J82" s="16"/>
     </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E83" s="1" t="s">
         <v>369</v>
       </c>
@@ -6669,7 +6677,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E84" s="1" t="s">
         <v>371</v>
       </c>
@@ -6687,7 +6695,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G85" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -6699,7 +6707,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E86" s="1" t="s">
         <v>374</v>
       </c>
@@ -6717,7 +6725,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E87" s="1" t="s">
         <v>376</v>
       </c>
@@ -6735,7 +6743,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E88" s="1" t="s">
         <v>378</v>
       </c>
@@ -6753,7 +6761,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D89" s="5" t="s">
         <v>390</v>
       </c>
@@ -6767,7 +6775,7 @@
       <c r="L89" s="5"/>
       <c r="M89" s="5"/>
     </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E90" s="1" t="s">
         <v>391</v>
       </c>
@@ -6785,7 +6793,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E91" s="1" t="s">
         <v>393</v>
       </c>
@@ -6803,7 +6811,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E92" s="1" t="s">
         <v>395</v>
       </c>
@@ -6821,7 +6829,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E93" s="1" t="s">
         <v>397</v>
       </c>
@@ -6839,7 +6847,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E94" s="1" t="s">
         <v>399</v>
       </c>
@@ -6857,7 +6865,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E95" s="1" t="s">
         <v>438</v>
       </c>
@@ -6875,7 +6883,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E96" s="1" t="s">
         <v>402</v>
       </c>
@@ -6893,7 +6901,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G97" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -6905,7 +6913,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E98" s="1" t="s">
         <v>405</v>
       </c>
@@ -6923,7 +6931,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E99" s="1" t="s">
         <v>407</v>
       </c>
@@ -6941,7 +6949,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E100" s="1" t="s">
         <v>409</v>
       </c>
@@ -6959,7 +6967,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E101" s="1" t="s">
         <v>411</v>
       </c>
@@ -6980,12 +6988,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J102" s="16" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E103" s="1" t="s">
         <v>413</v>
       </c>
@@ -7003,7 +7011,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E104" s="1" t="s">
         <v>415</v>
       </c>
@@ -7021,7 +7029,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H105" t="s">
         <v>417</v>
       </c>
@@ -7029,7 +7037,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E106" s="1" t="s">
         <v>418</v>
       </c>
@@ -7047,7 +7055,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G107" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7059,7 +7067,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E108" s="1" t="s">
         <v>421</v>
       </c>
@@ -7077,7 +7085,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H109" t="s">
         <v>423</v>
       </c>
@@ -7085,7 +7093,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="110" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E110" s="1" t="s">
         <v>424</v>
       </c>
@@ -7103,7 +7111,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="111" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E111" s="1" t="s">
         <v>426</v>
       </c>
@@ -7124,7 +7132,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="112" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:10" x14ac:dyDescent="0.45">
       <c r="F112" t="s">
         <v>433</v>
       </c>
@@ -7135,12 +7143,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="113" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J113" s="16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="114" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E114" s="1" t="s">
         <v>429</v>
       </c>
@@ -7158,7 +7166,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="115" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E115" s="1" t="s">
         <v>431</v>
       </c>
@@ -7179,7 +7187,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="116" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J116" s="16" t="s">
         <v>487</v>
       </c>
@@ -7195,22 +7203,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="48.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="31" t="s">
         <v>509</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="32" t="s">
+        <v>574</v>
+      </c>
       <c r="C2" s="32" t="s">
         <v>522</v>
       </c>
@@ -7225,7 +7235,7 @@
       </c>
       <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>510</v>
       </c>
@@ -7236,7 +7246,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="25"/>
       <c r="B4" s="26" t="s">
         <v>525</v>
@@ -7249,7 +7259,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="25"/>
       <c r="B5" s="26" t="s">
         <v>528</v>
@@ -7262,7 +7272,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="25"/>
       <c r="B6" s="26" t="s">
         <v>533</v>
@@ -7277,7 +7287,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="25"/>
       <c r="B7" s="26" t="s">
         <v>534</v>
@@ -7292,7 +7302,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="23"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7301,7 +7311,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>511</v>
       </c>
@@ -7312,7 +7322,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="25"/>
       <c r="B10" s="26" t="s">
         <v>535</v>
@@ -7325,7 +7335,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="24"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="s">
         <v>536</v>
@@ -7338,7 +7348,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="s">
         <v>537</v>
@@ -7351,7 +7361,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="s">
         <v>538</v>
@@ -7364,7 +7374,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="23"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7373,7 +7383,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>512</v>
       </c>
@@ -7384,7 +7394,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="25"/>
       <c r="B16" s="26" t="s">
         <v>540</v>
@@ -7399,7 +7409,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="25"/>
       <c r="B17" s="26" t="s">
         <v>543</v>
@@ -7412,7 +7422,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="25"/>
       <c r="B18" s="26" t="s">
         <v>544</v>
@@ -7425,7 +7435,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="23"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7434,7 +7444,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>513</v>
       </c>
@@ -7445,7 +7455,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="25"/>
       <c r="B21" s="26" t="s">
         <v>545</v>
@@ -7458,7 +7468,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="25"/>
       <c r="B22" s="26" t="s">
         <v>546</v>
@@ -7471,7 +7481,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="25"/>
       <c r="B23" s="26" t="s">
         <v>547</v>
@@ -7484,7 +7494,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -7493,7 +7503,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -7502,7 +7512,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>514</v>
       </c>
@@ -7513,7 +7523,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="25"/>
       <c r="B27" s="26" t="s">
         <v>548</v>
@@ -7526,7 +7536,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="25"/>
       <c r="B28" s="26" t="s">
         <v>550</v>
@@ -7539,7 +7549,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="25"/>
       <c r="B29" s="26" t="s">
         <v>551</v>
@@ -7552,7 +7562,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -7561,7 +7571,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="24"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
         <v>553</v>
       </c>
@@ -7574,7 +7584,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="25"/>
       <c r="B32" s="26" t="s">
         <v>555</v>
@@ -7587,7 +7597,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="25"/>
       <c r="B33" s="26" t="s">
         <v>556</v>
@@ -7600,7 +7610,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="25"/>
       <c r="B34" s="26" t="s">
         <v>557</v>
@@ -7615,7 +7625,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="23"/>
       <c r="B35" s="26" t="s">
         <v>558</v>
@@ -7628,7 +7638,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="24"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="26" t="s">
         <v>559</v>
@@ -7641,7 +7651,7 @@
       <c r="F36" s="8"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>561</v>
@@ -7654,7 +7664,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="23" t="s">
         <v>515</v>
       </c>
@@ -7665,7 +7675,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="25"/>
       <c r="B39" s="26" t="s">
         <v>562</v>
@@ -7678,7 +7688,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="24"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="25"/>
       <c r="B40" s="26" t="s">
         <v>563</v>
@@ -7691,7 +7701,7 @@
       <c r="F40" s="8"/>
       <c r="G40" s="24"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="25"/>
       <c r="B41" s="26" t="s">
         <v>564</v>
@@ -7704,123 +7714,205 @@
       <c r="F41" s="8"/>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
-      <c r="B42" s="28" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="25"/>
+      <c r="B42" s="26" t="s">
         <v>565</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29" t="s">
+      <c r="C42" s="8"/>
+      <c r="D42" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="23"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="23" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="20" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="25"/>
+      <c r="B45" s="26" t="s">
         <v>566</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B46" s="20" t="s">
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="25"/>
+      <c r="B46" s="26" t="s">
         <v>567</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" s="8"/>
+      <c r="D46" s="8" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="20" t="s">
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="25"/>
+      <c r="B47" s="26" t="s">
         <v>568</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="20" t="s">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="25"/>
+      <c r="B48" s="26" t="s">
         <v>569</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="24"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="23"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="24"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="23" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="20" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26" t="s">
         <v>570</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C51" s="8"/>
+      <c r="D51" s="8" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="20" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="24"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="25"/>
+      <c r="B52" s="26" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
+      <c r="C52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="24"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="23"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="24"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="23" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="20" t="s">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="24"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="25"/>
+      <c r="B55" s="26" t="s">
         <v>571</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C55" s="8"/>
+      <c r="D55" s="8" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="20" t="s">
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="24"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="25"/>
+      <c r="B56" s="26" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="20" t="s">
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="24"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="27"/>
+      <c r="B57" s="28" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="20" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="20" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="30"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B58" s="20"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B59" s="20"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="22"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(l17676) : docs 문서 수정
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="591">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3293,6 +3293,18 @@
   </si>
   <si>
     <t>현재 기준으로 before를 확인하는 방식으로 했으면 좀더 쉬웠을 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추석 트래픽(17676)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제 정확히 인지하지 못함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간내 못품</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7987,10 +7999,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H5"/>
+  <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8066,6 +8078,20 @@
         <v>587</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>588</v>
+      </c>
+      <c r="D6" t="s">
+        <v>589</v>
+      </c>
+      <c r="E6" t="s">
+        <v>590</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add(l17676) : 풀이 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="590">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3300,11 +3300,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>문제 정확히 인지하지 못함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시간내 못품</t>
+    <t>처음에 문제 정확히 인지하지 못함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7271,8 +7267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8002,7 +7998,7 @@
   <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8088,8 +8084,8 @@
       <c r="D6" t="s">
         <v>589</v>
       </c>
-      <c r="E6" t="s">
-        <v>590</v>
+      <c r="E6" s="8" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add(docs) : l72410 내용 추가
Signed-off-by: seongjin_song <seongjin_song@tmax.co.kr>
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="593">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3301,6 +3301,20 @@
   </si>
   <si>
     <t>처음에 문제 정확히 인지하지 못함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신규 아이디 추천(72410)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최적의 답으로 풀지 못함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 자바 스럽게 구현해보자
+2. 정규식 찾을 시간이 아까워 그냥 풀었다.
+&gt;&gt; 이정도는 정규식을 인지하고 있는게 나은가 생각도 들었다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7995,10 +8009,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8088,6 +8102,20 @@
         <v>560</v>
       </c>
     </row>
+    <row r="7" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>590</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>591</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add(l42888) : 간단한 hashmap 문제
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="596">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3315,6 +3315,18 @@
     <t>1. 자바 스럽게 구현해보자
 2. 정규식 찾을 시간이 아까워 그냥 풀었다.
 &gt;&gt; 이정도는 정규식을 인지하고 있는게 나은가 생각도 들었다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오픈채팅방(42888)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완벽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브라이언의 고민(1830)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8009,10 +8021,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8116,6 +8128,25 @@
         <v>591</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>593</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>595</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add(l81301) : 문제 해결
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="601">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3327,6 +3327,26 @@
   </si>
   <si>
     <t>브라이언의 고민(1830)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>못품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LinkedHashMap으로 HashMap에서도 순서를 가질 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자 문자열과 영단어(81301)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완벽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카카오프렌즈 컬러링북(1829)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8021,10 +8041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8146,6 +8166,31 @@
       <c r="C9" t="s">
         <v>595</v>
       </c>
+      <c r="D9" t="s">
+        <v>597</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>600</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add(l1829) : 문제 풀기
Signed-off-by: seongjin_song <seongjin_song@tmax.co.kr>
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="602">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3347,6 +3347,10 @@
   </si>
   <si>
     <t>카카오프렌즈 컬러링북(1829)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완벽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8044,7 +8048,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8191,6 +8195,9 @@
       <c r="C11" t="s">
         <v>600</v>
       </c>
+      <c r="E11" s="10" t="s">
+        <v>601</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix(l1836) : 풀이 완료
- 알파벳 순서대로 나오는 알고리즘을 이중포문으로 해결했는데 더 좋은
방법이 있는지
- 짝을 찾아가는 과정에서 ㄴ ㄱ 방식을 나눠서 검색했는데 더 좋은 길찾기
알고리즘이 있는지
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="603">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3351,6 +3351,10 @@
   </si>
   <si>
     <t>완벽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리틀 프렌즈 사천성(1836)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8045,10 +8049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8199,6 +8203,14 @@
         <v>601</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>602</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
docs : l1836 업데이트
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeongJin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="605">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3355,6 +3355,14 @@
   </si>
   <si>
     <t>리틀 프렌즈 사천성(1836)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간이 걸렸지만 풀음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 사람 정답이랑 비교는 안해봄</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8052,7 +8060,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8210,6 +8218,12 @@
       <c r="C12" t="s">
         <v>602</v>
       </c>
+      <c r="D12" t="s">
+        <v>604</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>603</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add(l77486): 문제 풀이 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjshi\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="9980" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="607">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3363,6 +3363,14 @@
   </si>
   <si>
     <t>다른 사람 정답이랑 비교는 안해봄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다단계 칫솔 판매(77486)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완벽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3964,27 +3972,27 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="3.625" customWidth="1"/>
-    <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="1" max="2" width="3.58203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.58203125" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.25" customWidth="1"/>
-    <col min="11" max="11" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.45">
       <c r="I3" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4016,7 +4024,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>172</v>
       </c>
@@ -4040,7 +4048,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4058,7 +4066,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -4076,7 +4084,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
@@ -4097,7 +4105,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
@@ -4118,7 +4126,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -4139,7 +4147,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
@@ -4157,7 +4165,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -4185,7 +4193,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
@@ -4203,7 +4211,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -4219,7 +4227,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -4235,7 +4243,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4256,7 +4264,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -4272,7 +4280,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E18" s="2"/>
       <c r="H18" t="s">
         <v>28</v>
@@ -4284,7 +4292,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
@@ -4302,7 +4310,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" ht="68.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D20" s="5" t="s">
         <v>202</v>
       </c>
@@ -4328,7 +4336,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4346,7 +4354,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
@@ -4364,7 +4372,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
@@ -4382,7 +4390,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4403,7 +4411,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -4419,7 +4427,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
@@ -4440,7 +4448,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -4461,7 +4469,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4482,7 +4490,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D29" s="5" t="s">
         <v>199</v>
       </c>
@@ -4508,7 +4516,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="4:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="68" x14ac:dyDescent="0.45">
       <c r="D30" s="8"/>
       <c r="E30" s="9" t="s">
         <v>204</v>
@@ -4532,7 +4540,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="4:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" ht="119" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -4556,7 +4564,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -4577,7 +4585,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>51</v>
       </c>
@@ -4598,7 +4606,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
@@ -4616,7 +4624,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -4637,7 +4645,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:12" ht="34.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>201</v>
       </c>
@@ -4663,7 +4671,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -4684,7 +4692,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
@@ -4706,7 +4714,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E39" s="1" t="s">
         <v>61</v>
       </c>
@@ -4721,7 +4729,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E40" s="2"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -4731,7 +4739,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
@@ -4746,7 +4754,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>64</v>
       </c>
@@ -4761,7 +4769,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E43" s="2"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -4771,7 +4779,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
@@ -4786,7 +4794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E45" s="1" t="s">
         <v>69</v>
       </c>
@@ -4801,7 +4809,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E46" s="2"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -4811,7 +4819,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
@@ -4826,7 +4834,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>74</v>
       </c>
@@ -4841,7 +4849,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E49" s="2"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -4851,7 +4859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E50" s="1" t="s">
         <v>77</v>
       </c>
@@ -4866,7 +4874,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E51" s="2"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -4876,7 +4884,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>80</v>
       </c>
@@ -4891,7 +4899,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E53" s="2"/>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -4901,7 +4909,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
@@ -4916,7 +4924,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E55" s="2"/>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -4926,7 +4934,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E56" s="1" t="s">
         <v>86</v>
       </c>
@@ -4941,7 +4949,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E57" s="1"/>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -4951,7 +4959,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D58" s="5" t="s">
         <v>89</v>
       </c>
@@ -4977,7 +4985,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>92</v>
       </c>
@@ -5001,7 +5009,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E60" t="s">
         <v>221</v>
       </c>
@@ -5015,7 +5023,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.45">
       <c r="H61" t="s">
         <v>95</v>
       </c>
@@ -5026,7 +5034,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
@@ -5047,7 +5055,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
@@ -5068,7 +5076,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>100</v>
       </c>
@@ -5086,7 +5094,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E65" t="s">
         <v>103</v>
       </c>
@@ -5101,7 +5109,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>104</v>
       </c>
@@ -5119,7 +5127,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>106</v>
       </c>
@@ -5137,7 +5145,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -5158,7 +5166,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
@@ -5179,7 +5187,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>112</v>
       </c>
@@ -5200,7 +5208,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>114</v>
       </c>
@@ -5224,7 +5232,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
         <v>117</v>
       </c>
@@ -5242,7 +5250,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
@@ -5260,7 +5268,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
         <v>121</v>
       </c>
@@ -5271,7 +5279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E75" s="1" t="s">
         <v>122</v>
       </c>
@@ -5295,7 +5303,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="76" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E76" s="1" t="s">
         <v>124</v>
       </c>
@@ -5319,25 +5327,25 @@
         <v>235</v>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E183" t="str">
         <f>IF(D183="","",CONCATENATE("https://www.acmicpc.net/problem/",D183))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E184" t="str">
         <f>IF(D184="","",CONCATENATE("https://www.acmicpc.net/problem/",D184))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E185" t="str">
         <f>IF(D185="","",CONCATENATE("https://www.acmicpc.net/problem/",D185))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E186" t="str">
         <f>IF(D186="","",CONCATENATE("https://www.acmicpc.net/problem/",D186))</f>
         <v/>
@@ -5358,22 +5366,22 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="22.75" customWidth="1"/>
-    <col min="5" max="5" width="26.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08203125" customWidth="1"/>
     <col min="7" max="7" width="37.5" customWidth="1"/>
     <col min="8" max="8" width="62" customWidth="1"/>
     <col min="9" max="9" width="9.75" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="62.875" customWidth="1"/>
-    <col min="12" max="12" width="34.875" customWidth="1"/>
+    <col min="11" max="11" width="62.83203125" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" customWidth="1"/>
     <col min="13" max="13" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.45">
       <c r="J2" s="1" t="s">
         <v>278</v>
       </c>
@@ -5381,7 +5389,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -5416,7 +5424,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>249</v>
       </c>
@@ -5424,7 +5432,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="99" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="102" x14ac:dyDescent="0.45">
       <c r="E5" s="14" t="s">
         <v>257</v>
       </c>
@@ -5451,7 +5459,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" ht="51" x14ac:dyDescent="0.45">
       <c r="E6" s="14" t="s">
         <v>258</v>
       </c>
@@ -5468,7 +5476,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>128</v>
       </c>
@@ -5492,7 +5500,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>130</v>
       </c>
@@ -5516,7 +5524,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>132</v>
       </c>
@@ -5537,7 +5545,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>134</v>
       </c>
@@ -5558,7 +5566,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>136</v>
       </c>
@@ -5579,7 +5587,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
@@ -5600,7 +5608,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>140</v>
       </c>
@@ -5621,7 +5629,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>142</v>
       </c>
@@ -5642,7 +5650,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E15" s="1" t="s">
         <v>144</v>
       </c>
@@ -5663,7 +5671,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>146</v>
       </c>
@@ -5687,7 +5695,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E17" s="1" t="s">
         <v>148</v>
       </c>
@@ -5708,7 +5716,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
@@ -5732,7 +5740,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E19" s="1" t="s">
         <v>153</v>
       </c>
@@ -5756,7 +5764,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="20" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E20" s="1" t="s">
         <v>154</v>
       </c>
@@ -5780,7 +5788,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>156</v>
       </c>
@@ -5801,7 +5809,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>158</v>
       </c>
@@ -5822,7 +5830,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="23" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="H23" t="s">
         <v>160</v>
       </c>
@@ -5836,7 +5844,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:11" ht="68" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
@@ -5860,7 +5868,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="H25" t="s">
         <v>162</v>
       </c>
@@ -5874,7 +5882,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>163</v>
       </c>
@@ -5895,7 +5903,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>165</v>
       </c>
@@ -5919,7 +5927,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E28" s="1" t="s">
         <v>167</v>
       </c>
@@ -5940,7 +5948,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E29" s="1" t="s">
         <v>169</v>
       </c>
@@ -5964,7 +5972,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H30" t="s">
         <v>171</v>
       </c>
@@ -5975,7 +5983,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>245</v>
       </c>
@@ -5999,7 +6007,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H32" t="s">
         <v>246</v>
       </c>
@@ -6010,7 +6018,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>243</v>
       </c>
@@ -6034,7 +6042,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>240</v>
       </c>
@@ -6055,7 +6063,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="35" spans="4:13" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:13" ht="51.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>239</v>
       </c>
@@ -6079,7 +6087,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>250</v>
       </c>
@@ -6093,7 +6101,7 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E37" s="15" t="s">
         <v>251</v>
       </c>
@@ -6111,7 +6119,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H38" t="s">
         <v>253</v>
       </c>
@@ -6119,7 +6127,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H39" t="s">
         <v>254</v>
       </c>
@@ -6127,7 +6135,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H40" t="s">
         <v>255</v>
       </c>
@@ -6135,7 +6143,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H41" t="s">
         <v>290</v>
       </c>
@@ -6143,7 +6151,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>292</v>
       </c>
@@ -6161,7 +6169,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H43" t="s">
         <v>294</v>
       </c>
@@ -6169,7 +6177,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E44" s="14" t="s">
         <v>309</v>
       </c>
@@ -6187,7 +6195,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="45" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E45" s="14" t="s">
         <v>307</v>
       </c>
@@ -6198,7 +6206,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E46" s="1" t="s">
         <v>300</v>
       </c>
@@ -6216,7 +6224,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>301</v>
       </c>
@@ -6234,7 +6242,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>303</v>
       </c>
@@ -6252,7 +6260,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="49" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E49" s="14" t="s">
         <v>308</v>
       </c>
@@ -6270,7 +6278,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="50" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E50" s="14" t="s">
         <v>310</v>
       </c>
@@ -6281,7 +6289,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E51" s="1" t="s">
         <v>312</v>
       </c>
@@ -6299,7 +6307,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>314</v>
       </c>
@@ -6317,7 +6325,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E53" s="1" t="s">
         <v>316</v>
       </c>
@@ -6335,7 +6343,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>318</v>
       </c>
@@ -6353,7 +6361,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E55" s="1" t="s">
         <v>320</v>
       </c>
@@ -6371,7 +6379,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H56" t="s">
         <v>322</v>
       </c>
@@ -6379,7 +6387,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E57" s="1" t="s">
         <v>323</v>
       </c>
@@ -6397,7 +6405,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E58" s="1" t="s">
         <v>326</v>
       </c>
@@ -6415,7 +6423,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>327</v>
       </c>
@@ -6433,7 +6441,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E60" s="1" t="s">
         <v>329</v>
       </c>
@@ -6451,7 +6459,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="61" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E61" s="1" t="s">
         <v>331</v>
       </c>
@@ -6469,7 +6477,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="62" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D62" s="5" t="s">
         <v>333</v>
       </c>
@@ -6483,7 +6491,7 @@
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
     </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>243</v>
       </c>
@@ -6501,7 +6509,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>335</v>
       </c>
@@ -6519,7 +6527,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E65" s="1" t="s">
         <v>337</v>
       </c>
@@ -6537,7 +6545,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>339</v>
       </c>
@@ -6555,7 +6563,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>142</v>
       </c>
@@ -6570,7 +6578,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>341</v>
       </c>
@@ -6588,7 +6596,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>343</v>
       </c>
@@ -6606,7 +6614,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>345</v>
       </c>
@@ -6624,7 +6632,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>347</v>
       </c>
@@ -6642,7 +6650,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E72" s="1" t="s">
         <v>349</v>
       </c>
@@ -6660,7 +6668,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H73" t="s">
         <v>355</v>
       </c>
@@ -6668,7 +6676,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H74" t="s">
         <v>356</v>
       </c>
@@ -6676,7 +6684,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H75" t="s">
         <v>357</v>
       </c>
@@ -6684,7 +6692,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="H76" t="s">
         <v>358</v>
       </c>
@@ -6692,7 +6700,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D77" s="5" t="s">
         <v>359</v>
       </c>
@@ -6706,7 +6714,7 @@
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E78" s="1" t="s">
         <v>361</v>
       </c>
@@ -6724,7 +6732,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E79" s="1" t="s">
         <v>363</v>
       </c>
@@ -6742,7 +6750,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E80" s="1" t="s">
         <v>365</v>
       </c>
@@ -6760,7 +6768,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G81" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -6772,7 +6780,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E82" s="1" t="s">
         <v>366</v>
       </c>
@@ -6785,7 +6793,7 @@
       </c>
       <c r="J82" s="16"/>
     </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E83" s="1" t="s">
         <v>369</v>
       </c>
@@ -6803,7 +6811,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E84" s="1" t="s">
         <v>371</v>
       </c>
@@ -6821,7 +6829,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G85" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -6833,7 +6841,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E86" s="1" t="s">
         <v>374</v>
       </c>
@@ -6851,7 +6859,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E87" s="1" t="s">
         <v>376</v>
       </c>
@@ -6869,7 +6877,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E88" s="1" t="s">
         <v>378</v>
       </c>
@@ -6887,7 +6895,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D89" s="5" t="s">
         <v>390</v>
       </c>
@@ -6901,7 +6909,7 @@
       <c r="L89" s="5"/>
       <c r="M89" s="5"/>
     </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E90" s="1" t="s">
         <v>391</v>
       </c>
@@ -6919,7 +6927,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E91" s="1" t="s">
         <v>393</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E92" s="1" t="s">
         <v>395</v>
       </c>
@@ -6955,7 +6963,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E93" s="1" t="s">
         <v>397</v>
       </c>
@@ -6973,7 +6981,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E94" s="1" t="s">
         <v>399</v>
       </c>
@@ -6991,7 +6999,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E95" s="1" t="s">
         <v>438</v>
       </c>
@@ -7009,7 +7017,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E96" s="1" t="s">
         <v>402</v>
       </c>
@@ -7027,7 +7035,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G97" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7039,7 +7047,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E98" s="1" t="s">
         <v>405</v>
       </c>
@@ -7057,7 +7065,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E99" s="1" t="s">
         <v>407</v>
       </c>
@@ -7075,7 +7083,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E100" s="1" t="s">
         <v>409</v>
       </c>
@@ -7093,7 +7101,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E101" s="1" t="s">
         <v>411</v>
       </c>
@@ -7114,12 +7122,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J102" s="16" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E103" s="1" t="s">
         <v>413</v>
       </c>
@@ -7137,7 +7145,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E104" s="1" t="s">
         <v>415</v>
       </c>
@@ -7155,7 +7163,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H105" t="s">
         <v>417</v>
       </c>
@@ -7163,7 +7171,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E106" s="1" t="s">
         <v>418</v>
       </c>
@@ -7181,7 +7189,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G107" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7193,7 +7201,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E108" s="1" t="s">
         <v>421</v>
       </c>
@@ -7211,7 +7219,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H109" t="s">
         <v>423</v>
       </c>
@@ -7219,7 +7227,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="110" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E110" s="1" t="s">
         <v>424</v>
       </c>
@@ -7237,7 +7245,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="111" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E111" s="1" t="s">
         <v>426</v>
       </c>
@@ -7258,7 +7266,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="112" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:10" x14ac:dyDescent="0.45">
       <c r="F112" t="s">
         <v>433</v>
       </c>
@@ -7269,12 +7277,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="113" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J113" s="16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="114" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E114" s="1" t="s">
         <v>429</v>
       </c>
@@ -7292,7 +7300,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="115" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E115" s="1" t="s">
         <v>431</v>
       </c>
@@ -7313,7 +7321,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="116" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J116" s="16" t="s">
         <v>487</v>
       </c>
@@ -7333,15 +7341,15 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.75" customWidth="1"/>
     <col min="2" max="2" width="25.25" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="22.375" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="31" t="s">
         <v>509</v>
       </c>
@@ -7362,7 +7370,7 @@
       </c>
       <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>510</v>
       </c>
@@ -7373,7 +7381,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="25"/>
       <c r="B4" s="26" t="s">
         <v>525</v>
@@ -7386,7 +7394,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="25"/>
       <c r="B5" s="26" t="s">
         <v>528</v>
@@ -7399,7 +7407,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="25"/>
       <c r="B6" s="26" t="s">
         <v>533</v>
@@ -7414,7 +7422,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="25"/>
       <c r="B7" s="26" t="s">
         <v>534</v>
@@ -7429,7 +7437,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="23"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7438,7 +7446,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>511</v>
       </c>
@@ -7449,7 +7457,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="25"/>
       <c r="B10" s="26" t="s">
         <v>535</v>
@@ -7462,7 +7470,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="24"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="s">
         <v>536</v>
@@ -7475,7 +7483,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="s">
         <v>537</v>
@@ -7488,7 +7496,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="s">
         <v>538</v>
@@ -7501,7 +7509,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="23"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7510,7 +7518,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>512</v>
       </c>
@@ -7521,7 +7529,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="25"/>
       <c r="B16" s="26" t="s">
         <v>540</v>
@@ -7536,7 +7544,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="25"/>
       <c r="B17" s="26" t="s">
         <v>543</v>
@@ -7549,7 +7557,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="25"/>
       <c r="B18" s="26" t="s">
         <v>544</v>
@@ -7562,7 +7570,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="23"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7571,7 +7579,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>513</v>
       </c>
@@ -7582,7 +7590,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="25"/>
       <c r="B21" s="26" t="s">
         <v>545</v>
@@ -7595,7 +7603,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="25"/>
       <c r="B22" s="26" t="s">
         <v>546</v>
@@ -7608,7 +7616,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="25"/>
       <c r="B23" s="26" t="s">
         <v>547</v>
@@ -7621,7 +7629,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -7630,7 +7638,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -7639,7 +7647,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>514</v>
       </c>
@@ -7650,7 +7658,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="25"/>
       <c r="B27" s="26" t="s">
         <v>548</v>
@@ -7663,7 +7671,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="25"/>
       <c r="B28" s="26" t="s">
         <v>550</v>
@@ -7676,7 +7684,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="25"/>
       <c r="B29" s="26" t="s">
         <v>551</v>
@@ -7689,7 +7697,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -7698,7 +7706,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="24"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
         <v>553</v>
       </c>
@@ -7711,7 +7719,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="25"/>
       <c r="B32" s="26" t="s">
         <v>555</v>
@@ -7724,7 +7732,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="25"/>
       <c r="B33" s="26" t="s">
         <v>556</v>
@@ -7737,7 +7745,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="25"/>
       <c r="B34" s="26" t="s">
         <v>557</v>
@@ -7752,7 +7760,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="23"/>
       <c r="B35" s="26" t="s">
         <v>558</v>
@@ -7765,7 +7773,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="24"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="26" t="s">
         <v>559</v>
@@ -7778,7 +7786,7 @@
       <c r="F36" s="8"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>561</v>
@@ -7791,7 +7799,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="23" t="s">
         <v>515</v>
       </c>
@@ -7802,7 +7810,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="25"/>
       <c r="B39" s="26" t="s">
         <v>562</v>
@@ -7815,7 +7823,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="24"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="25"/>
       <c r="B40" s="26" t="s">
         <v>563</v>
@@ -7828,7 +7836,7 @@
       <c r="F40" s="8"/>
       <c r="G40" s="24"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="25"/>
       <c r="B41" s="26" t="s">
         <v>564</v>
@@ -7841,7 +7849,7 @@
       <c r="F41" s="8"/>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="25"/>
       <c r="B42" s="26" t="s">
         <v>565</v>
@@ -7854,7 +7862,7 @@
       <c r="F42" s="8"/>
       <c r="G42" s="24"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="23"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -7863,7 +7871,7 @@
       <c r="F43" s="8"/>
       <c r="G43" s="24"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="23" t="s">
         <v>516</v>
       </c>
@@ -7874,7 +7882,7 @@
       <c r="F44" s="8"/>
       <c r="G44" s="24"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="25"/>
       <c r="B45" s="26" t="s">
         <v>566</v>
@@ -7887,7 +7895,7 @@
       <c r="F45" s="8"/>
       <c r="G45" s="24"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="25"/>
       <c r="B46" s="26" t="s">
         <v>567</v>
@@ -7900,7 +7908,7 @@
       <c r="F46" s="8"/>
       <c r="G46" s="24"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="25"/>
       <c r="B47" s="26" t="s">
         <v>568</v>
@@ -7913,7 +7921,7 @@
       <c r="F47" s="8"/>
       <c r="G47" s="24"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="25"/>
       <c r="B48" s="26" t="s">
         <v>569</v>
@@ -7926,7 +7934,7 @@
       <c r="F48" s="8"/>
       <c r="G48" s="24"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="23"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -7935,7 +7943,7 @@
       <c r="F49" s="8"/>
       <c r="G49" s="24"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>517</v>
       </c>
@@ -7946,7 +7954,7 @@
       <c r="F50" s="8"/>
       <c r="G50" s="24"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="25"/>
       <c r="B51" s="26" t="s">
         <v>570</v>
@@ -7961,7 +7969,7 @@
       <c r="F51" s="8"/>
       <c r="G51" s="24"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="25"/>
       <c r="B52" s="26" t="s">
         <v>518</v>
@@ -7974,7 +7982,7 @@
       <c r="F52" s="8"/>
       <c r="G52" s="24"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -7983,7 +7991,7 @@
       <c r="F53" s="8"/>
       <c r="G53" s="24"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>519</v>
       </c>
@@ -7994,7 +8002,7 @@
       <c r="F54" s="8"/>
       <c r="G54" s="24"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="25"/>
       <c r="B55" s="26" t="s">
         <v>571</v>
@@ -8007,7 +8015,7 @@
       <c r="F55" s="8"/>
       <c r="G55" s="24"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="25"/>
       <c r="B56" s="26" t="s">
         <v>520</v>
@@ -8022,7 +8030,7 @@
       <c r="F56" s="8"/>
       <c r="G56" s="24"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="27"/>
       <c r="B57" s="28" t="s">
         <v>521</v>
@@ -8033,19 +8041,19 @@
       <c r="F57" s="29"/>
       <c r="G57" s="30"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B58" s="20"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B59" s="20"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="22"/>
     </row>
   </sheetData>
@@ -8057,22 +8065,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H12"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="27.08203125" customWidth="1"/>
     <col min="2" max="2" width="9.75" customWidth="1"/>
-    <col min="3" max="3" width="60.375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="4" width="70.75" customWidth="1"/>
-    <col min="5" max="5" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
         <v>580</v>
       </c>
@@ -8096,7 +8104,7 @@
       </c>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
       <c r="B3" s="26">
         <v>1</v>
@@ -8114,7 +8122,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2</v>
       </c>
@@ -8128,7 +8136,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>585</v>
       </c>
@@ -8136,7 +8144,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>3</v>
       </c>
@@ -8150,7 +8158,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1</v>
       </c>
@@ -8164,7 +8172,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>2</v>
       </c>
@@ -8175,7 +8183,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>3</v>
       </c>
@@ -8189,7 +8197,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>1</v>
       </c>
@@ -8200,7 +8208,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>2</v>
       </c>
@@ -8211,7 +8219,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>3</v>
       </c>
@@ -8223,6 +8231,17 @@
       </c>
       <c r="E12" s="10" t="s">
         <v>603</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>605</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add(l12973): 문제 푸는 중
성능테스트에서 막힘
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="624">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3438,6 +3438,14 @@
   <si>
     <t>3진수로 접근하는건 알았는데 n-1/3 처리를 못찾아냄
 sb.insert 함수로 prepend 처리가 가능하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짝지어 제거하기(12973)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성능 못통과</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8178,10 +8186,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H18"/>
+  <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8427,6 +8435,17 @@
         <v>620</v>
       </c>
     </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>622</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>623</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add(l12977) : 성능 제외 통과
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="639">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3502,6 +3502,14 @@
   <si>
     <t>두번 읽어봤는데 문제가 이해가 안간다
 앱출력 예제중 2번, 6번 이해가 안간다;;;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소수 만들기(12977)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1차 구현 성능 막힘</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8242,10 +8250,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8555,14 +8563,25 @@
         <v>633</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>637</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>635</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>636</v>
       </c>
     </row>

</xml_diff>

<commit_message>
complete - 19 test case(l17678)
19번 testCate 제외하고 완료

- IDE 사용 못하는 경우를 대비해서 java.text.* 잊지말자
- SimpleDateFormat을 이용해서 시간 연산을 하자
- 시간 연산이 필요한 경우 long 타입으로 연산하고 마지막에 String으로 변경하자!
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\Algorithm\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjshi\git\Algorithm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="9980" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="640">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3500,17 +3500,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>두번 읽어봤는데 문제가 이해가 안간다
-앱출력 예제중 2번, 6번 이해가 안간다;;;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>소수 만들기(12977)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3중포문으로 문제 풀 수 있다.
 Combination 구현하는걸 알아보자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문제 이해했다는 가정하에 시간내에 풀음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">두번 읽어봤는데 문제가 이해가 안간다
+앱출력 예제중 2번, 6번 이해가 안간다;;;
+&gt;&gt; 문제 이해가 좀 헷갈렷지만 이해만 하면 어렵지 않다.
+19번 테스트케이스만 통과가 안된다… 이유가 뭘까?ㅜㅜ
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4158,27 +4165,27 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="3.625" customWidth="1"/>
-    <col min="3" max="3" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="1" max="2" width="3.58203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.58203125" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
     <col min="8" max="8" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.25" customWidth="1"/>
-    <col min="11" max="11" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.45">
       <c r="I3" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4210,7 +4217,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>172</v>
       </c>
@@ -4234,7 +4241,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4252,7 +4259,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -4270,7 +4277,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
@@ -4291,7 +4298,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
@@ -4312,7 +4319,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
@@ -4333,7 +4340,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="3:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
@@ -4351,7 +4358,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="3:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5" t="s">
         <v>18</v>
       </c>
@@ -4379,7 +4386,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
@@ -4397,7 +4404,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -4413,7 +4420,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -4429,7 +4436,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4450,7 +4457,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E17" s="2"/>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -4466,7 +4473,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E18" s="2"/>
       <c r="H18" t="s">
         <v>28</v>
@@ -4478,7 +4485,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
@@ -4496,7 +4503,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="4:12" ht="66.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" ht="68.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D20" s="5" t="s">
         <v>202</v>
       </c>
@@ -4522,7 +4529,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4540,7 +4547,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
@@ -4558,7 +4565,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
@@ -4576,7 +4583,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4597,7 +4604,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -4613,7 +4620,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>42</v>
       </c>
@@ -4634,7 +4641,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -4655,7 +4662,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4676,7 +4683,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D29" s="5" t="s">
         <v>199</v>
       </c>
@@ -4702,7 +4709,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="4:12" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" ht="68" x14ac:dyDescent="0.45">
       <c r="D30" s="8"/>
       <c r="E30" s="9" t="s">
         <v>204</v>
@@ -4726,7 +4733,7 @@
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
     </row>
-    <row r="31" spans="4:12" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" ht="119" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -4750,7 +4757,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -4771,7 +4778,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>51</v>
       </c>
@@ -4792,7 +4799,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>48</v>
       </c>
@@ -4810,7 +4817,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="4:12" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>49</v>
       </c>
@@ -4831,7 +4838,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="4:12" ht="33.75" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:12" ht="34.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>201</v>
       </c>
@@ -4857,7 +4864,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -4878,7 +4885,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D38" s="5" t="s">
         <v>56</v>
       </c>
@@ -4900,7 +4907,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E39" s="1" t="s">
         <v>61</v>
       </c>
@@ -4915,7 +4922,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E40" s="2"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -4925,7 +4932,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
@@ -4940,7 +4947,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>64</v>
       </c>
@@ -4955,7 +4962,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E43" s="2"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -4965,7 +4972,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E44" s="1" t="s">
         <v>67</v>
       </c>
@@ -4980,7 +4987,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E45" s="1" t="s">
         <v>69</v>
       </c>
@@ -4995,7 +5002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E46" s="2"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -5005,7 +5012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
@@ -5020,7 +5027,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>74</v>
       </c>
@@ -5035,7 +5042,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E49" s="2"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -5045,7 +5052,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E50" s="1" t="s">
         <v>77</v>
       </c>
@@ -5060,7 +5067,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E51" s="2"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -5070,7 +5077,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>80</v>
       </c>
@@ -5085,7 +5092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E53" s="2"/>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -5095,7 +5102,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
@@ -5110,7 +5117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E55" s="2"/>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -5120,7 +5127,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E56" s="1" t="s">
         <v>86</v>
       </c>
@@ -5135,7 +5142,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="4:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E57" s="1"/>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -5145,7 +5152,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="4:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D58" s="5" t="s">
         <v>89</v>
       </c>
@@ -5171,7 +5178,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>92</v>
       </c>
@@ -5195,7 +5202,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="4:12" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:12" ht="51" x14ac:dyDescent="0.45">
       <c r="E60" t="s">
         <v>221</v>
       </c>
@@ -5209,7 +5216,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:12" x14ac:dyDescent="0.45">
       <c r="H61" t="s">
         <v>95</v>
       </c>
@@ -5220,7 +5227,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E62" s="1" t="s">
         <v>96</v>
       </c>
@@ -5241,7 +5248,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="4:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:12" ht="34" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
@@ -5262,7 +5269,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>100</v>
       </c>
@@ -5280,7 +5287,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E65" t="s">
         <v>103</v>
       </c>
@@ -5295,7 +5302,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>104</v>
       </c>
@@ -5313,7 +5320,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>106</v>
       </c>
@@ -5331,7 +5338,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -5352,7 +5359,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>110</v>
       </c>
@@ -5373,7 +5380,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>112</v>
       </c>
@@ -5394,7 +5401,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>114</v>
       </c>
@@ -5418,7 +5425,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E72" t="s">
         <v>117</v>
       </c>
@@ -5436,7 +5443,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E73" s="1" t="s">
         <v>118</v>
       </c>
@@ -5454,7 +5461,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E74" t="s">
         <v>121</v>
       </c>
@@ -5465,7 +5472,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="E75" s="1" t="s">
         <v>122</v>
       </c>
@@ -5489,7 +5496,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="76" spans="5:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:11" ht="85" x14ac:dyDescent="0.45">
       <c r="E76" s="1" t="s">
         <v>124</v>
       </c>
@@ -5513,25 +5520,25 @@
         <v>235</v>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E183" t="str">
         <f>IF(D183="","",CONCATENATE("https://www.acmicpc.net/problem/",D183))</f>
         <v/>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E184" t="str">
         <f>IF(D184="","",CONCATENATE("https://www.acmicpc.net/problem/",D184))</f>
         <v/>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E185" t="str">
         <f>IF(D185="","",CONCATENATE("https://www.acmicpc.net/problem/",D185))</f>
         <v/>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.45">
       <c r="E186" t="str">
         <f>IF(D186="","",CONCATENATE("https://www.acmicpc.net/problem/",D186))</f>
         <v/>
@@ -5552,22 +5559,22 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="42" customWidth="1"/>
     <col min="4" max="4" width="22.75" customWidth="1"/>
-    <col min="5" max="5" width="26.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.08203125" customWidth="1"/>
     <col min="7" max="7" width="37.5" customWidth="1"/>
     <col min="8" max="8" width="62" customWidth="1"/>
     <col min="9" max="9" width="9.75" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="62.875" customWidth="1"/>
-    <col min="12" max="12" width="34.875" customWidth="1"/>
+    <col min="11" max="11" width="62.83203125" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" customWidth="1"/>
     <col min="13" max="13" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.45">
       <c r="J2" s="1" t="s">
         <v>278</v>
       </c>
@@ -5575,7 +5582,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -5610,7 +5617,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>249</v>
       </c>
@@ -5618,7 +5625,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="99" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="102" x14ac:dyDescent="0.45">
       <c r="E5" s="14" t="s">
         <v>257</v>
       </c>
@@ -5645,7 +5652,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" ht="51" x14ac:dyDescent="0.45">
       <c r="E6" s="14" t="s">
         <v>258</v>
       </c>
@@ -5662,7 +5669,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E7" s="1" t="s">
         <v>128</v>
       </c>
@@ -5686,7 +5693,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E8" s="1" t="s">
         <v>130</v>
       </c>
@@ -5710,7 +5717,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>132</v>
       </c>
@@ -5731,7 +5738,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>134</v>
       </c>
@@ -5752,7 +5759,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>136</v>
       </c>
@@ -5773,7 +5780,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E12" s="1" t="s">
         <v>138</v>
       </c>
@@ -5794,7 +5801,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>140</v>
       </c>
@@ -5815,7 +5822,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>142</v>
       </c>
@@ -5836,7 +5843,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E15" s="1" t="s">
         <v>144</v>
       </c>
@@ -5857,7 +5864,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>146</v>
       </c>
@@ -5881,7 +5888,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E17" s="1" t="s">
         <v>148</v>
       </c>
@@ -5902,7 +5909,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
@@ -5926,7 +5933,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E19" s="1" t="s">
         <v>153</v>
       </c>
@@ -5950,7 +5957,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="20" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E20" s="1" t="s">
         <v>154</v>
       </c>
@@ -5974,7 +5981,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E21" s="1" t="s">
         <v>156</v>
       </c>
@@ -5995,7 +6002,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>158</v>
       </c>
@@ -6016,7 +6023,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="23" spans="5:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:11" ht="51" x14ac:dyDescent="0.45">
       <c r="H23" t="s">
         <v>160</v>
       </c>
@@ -6030,7 +6037,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="5:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:11" ht="68" x14ac:dyDescent="0.45">
       <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
@@ -6054,7 +6061,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="H25" t="s">
         <v>162</v>
       </c>
@@ -6068,7 +6075,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E26" s="1" t="s">
         <v>163</v>
       </c>
@@ -6089,7 +6096,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>165</v>
       </c>
@@ -6113,7 +6120,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E28" s="1" t="s">
         <v>167</v>
       </c>
@@ -6134,7 +6141,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E29" s="1" t="s">
         <v>169</v>
       </c>
@@ -6158,7 +6165,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H30" t="s">
         <v>171</v>
       </c>
@@ -6169,7 +6176,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="5:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:11" ht="34" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>245</v>
       </c>
@@ -6193,7 +6200,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.45">
       <c r="H32" t="s">
         <v>246</v>
       </c>
@@ -6204,7 +6211,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E33" s="1" t="s">
         <v>243</v>
       </c>
@@ -6228,7 +6235,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>240</v>
       </c>
@@ -6249,7 +6256,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="35" spans="4:13" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:13" ht="51.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="1" t="s">
         <v>239</v>
       </c>
@@ -6273,7 +6280,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D36" s="5" t="s">
         <v>250</v>
       </c>
@@ -6287,7 +6294,7 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E37" s="15" t="s">
         <v>251</v>
       </c>
@@ -6305,7 +6312,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H38" t="s">
         <v>253</v>
       </c>
@@ -6313,7 +6320,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H39" t="s">
         <v>254</v>
       </c>
@@ -6321,7 +6328,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H40" t="s">
         <v>255</v>
       </c>
@@ -6329,7 +6336,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H41" t="s">
         <v>290</v>
       </c>
@@ -6337,7 +6344,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E42" s="1" t="s">
         <v>292</v>
       </c>
@@ -6355,7 +6362,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H43" t="s">
         <v>294</v>
       </c>
@@ -6363,7 +6370,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E44" s="14" t="s">
         <v>309</v>
       </c>
@@ -6381,7 +6388,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="45" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E45" s="14" t="s">
         <v>307</v>
       </c>
@@ -6392,7 +6399,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E46" s="1" t="s">
         <v>300</v>
       </c>
@@ -6410,7 +6417,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E47" s="1" t="s">
         <v>301</v>
       </c>
@@ -6428,7 +6435,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E48" s="1" t="s">
         <v>303</v>
       </c>
@@ -6446,7 +6453,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="49" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E49" s="14" t="s">
         <v>308</v>
       </c>
@@ -6464,7 +6471,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="50" spans="4:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:13" ht="34" x14ac:dyDescent="0.45">
       <c r="E50" s="14" t="s">
         <v>310</v>
       </c>
@@ -6475,7 +6482,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E51" s="1" t="s">
         <v>312</v>
       </c>
@@ -6493,7 +6500,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E52" s="1" t="s">
         <v>314</v>
       </c>
@@ -6511,7 +6518,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E53" s="1" t="s">
         <v>316</v>
       </c>
@@ -6529,7 +6536,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E54" s="1" t="s">
         <v>318</v>
       </c>
@@ -6547,7 +6554,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E55" s="1" t="s">
         <v>320</v>
       </c>
@@ -6565,7 +6572,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H56" t="s">
         <v>322</v>
       </c>
@@ -6573,7 +6580,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E57" s="1" t="s">
         <v>323</v>
       </c>
@@ -6591,7 +6598,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E58" s="1" t="s">
         <v>326</v>
       </c>
@@ -6609,7 +6616,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E59" s="1" t="s">
         <v>327</v>
       </c>
@@ -6627,7 +6634,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E60" s="1" t="s">
         <v>329</v>
       </c>
@@ -6645,7 +6652,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="61" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E61" s="1" t="s">
         <v>331</v>
       </c>
@@ -6663,7 +6670,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="62" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D62" s="5" t="s">
         <v>333</v>
       </c>
@@ -6677,7 +6684,7 @@
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
     </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E63" s="1" t="s">
         <v>243</v>
       </c>
@@ -6695,7 +6702,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E64" s="1" t="s">
         <v>335</v>
       </c>
@@ -6713,7 +6720,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E65" s="1" t="s">
         <v>337</v>
       </c>
@@ -6731,7 +6738,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E66" s="1" t="s">
         <v>339</v>
       </c>
@@ -6749,7 +6756,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E67" s="1" t="s">
         <v>142</v>
       </c>
@@ -6764,7 +6771,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E68" s="1" t="s">
         <v>341</v>
       </c>
@@ -6782,7 +6789,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E69" s="1" t="s">
         <v>343</v>
       </c>
@@ -6800,7 +6807,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E70" s="1" t="s">
         <v>345</v>
       </c>
@@ -6818,7 +6825,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E71" s="1" t="s">
         <v>347</v>
       </c>
@@ -6836,7 +6843,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E72" s="1" t="s">
         <v>349</v>
       </c>
@@ -6854,7 +6861,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H73" t="s">
         <v>355</v>
       </c>
@@ -6862,7 +6869,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H74" t="s">
         <v>356</v>
       </c>
@@ -6870,7 +6877,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:13" x14ac:dyDescent="0.45">
       <c r="H75" t="s">
         <v>357</v>
       </c>
@@ -6878,7 +6885,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="H76" t="s">
         <v>358</v>
       </c>
@@ -6886,7 +6893,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D77" s="5" t="s">
         <v>359</v>
       </c>
@@ -6900,7 +6907,7 @@
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E78" s="1" t="s">
         <v>361</v>
       </c>
@@ -6918,7 +6925,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E79" s="1" t="s">
         <v>363</v>
       </c>
@@ -6936,7 +6943,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E80" s="1" t="s">
         <v>365</v>
       </c>
@@ -6954,7 +6961,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="81" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G81" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -6966,7 +6973,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="82" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E82" s="1" t="s">
         <v>366</v>
       </c>
@@ -6979,7 +6986,7 @@
       </c>
       <c r="J82" s="16"/>
     </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E83" s="1" t="s">
         <v>369</v>
       </c>
@@ -6997,7 +7004,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E84" s="1" t="s">
         <v>371</v>
       </c>
@@ -7015,7 +7022,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:13" x14ac:dyDescent="0.45">
       <c r="G85" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7027,7 +7034,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E86" s="1" t="s">
         <v>374</v>
       </c>
@@ -7045,7 +7052,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E87" s="1" t="s">
         <v>376</v>
       </c>
@@ -7063,7 +7070,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="4:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E88" s="1" t="s">
         <v>378</v>
       </c>
@@ -7081,7 +7088,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="4:13" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D89" s="5" t="s">
         <v>390</v>
       </c>
@@ -7095,7 +7102,7 @@
       <c r="L89" s="5"/>
       <c r="M89" s="5"/>
     </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E90" s="1" t="s">
         <v>391</v>
       </c>
@@ -7113,7 +7120,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E91" s="1" t="s">
         <v>393</v>
       </c>
@@ -7131,7 +7138,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E92" s="1" t="s">
         <v>395</v>
       </c>
@@ -7149,7 +7156,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E93" s="1" t="s">
         <v>397</v>
       </c>
@@ -7167,7 +7174,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E94" s="1" t="s">
         <v>399</v>
       </c>
@@ -7185,7 +7192,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E95" s="1" t="s">
         <v>438</v>
       </c>
@@ -7203,7 +7210,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:13" x14ac:dyDescent="0.45">
       <c r="E96" s="1" t="s">
         <v>402</v>
       </c>
@@ -7221,7 +7228,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G97" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7233,7 +7240,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E98" s="1" t="s">
         <v>405</v>
       </c>
@@ -7251,7 +7258,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E99" s="1" t="s">
         <v>407</v>
       </c>
@@ -7269,7 +7276,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E100" s="1" t="s">
         <v>409</v>
       </c>
@@ -7287,7 +7294,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E101" s="1" t="s">
         <v>411</v>
       </c>
@@ -7308,12 +7315,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J102" s="16" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E103" s="1" t="s">
         <v>413</v>
       </c>
@@ -7331,7 +7338,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E104" s="1" t="s">
         <v>415</v>
       </c>
@@ -7349,7 +7356,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H105" t="s">
         <v>417</v>
       </c>
@@ -7357,7 +7364,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E106" s="1" t="s">
         <v>418</v>
       </c>
@@ -7375,7 +7382,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:10" x14ac:dyDescent="0.45">
       <c r="G107" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -7387,7 +7394,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E108" s="1" t="s">
         <v>421</v>
       </c>
@@ -7405,7 +7412,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:10" x14ac:dyDescent="0.45">
       <c r="H109" t="s">
         <v>423</v>
       </c>
@@ -7413,7 +7420,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="110" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E110" s="1" t="s">
         <v>424</v>
       </c>
@@ -7431,7 +7438,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="111" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E111" s="1" t="s">
         <v>426</v>
       </c>
@@ -7452,7 +7459,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="112" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:10" x14ac:dyDescent="0.45">
       <c r="F112" t="s">
         <v>433</v>
       </c>
@@ -7463,12 +7470,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="113" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J113" s="16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="114" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E114" s="1" t="s">
         <v>429</v>
       </c>
@@ -7486,7 +7493,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="115" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E115" s="1" t="s">
         <v>431</v>
       </c>
@@ -7507,7 +7514,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="116" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:10" x14ac:dyDescent="0.45">
       <c r="J116" s="16" t="s">
         <v>487</v>
       </c>
@@ -7527,15 +7534,15 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.75" customWidth="1"/>
     <col min="2" max="2" width="25.25" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="22.375" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="31" t="s">
         <v>509</v>
       </c>
@@ -7556,7 +7563,7 @@
       </c>
       <c r="G2" s="32"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>510</v>
       </c>
@@ -7567,7 +7574,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="24"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="25"/>
       <c r="B4" s="26" t="s">
         <v>525</v>
@@ -7580,7 +7587,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="25"/>
       <c r="B5" s="26" t="s">
         <v>528</v>
@@ -7593,7 +7600,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="25"/>
       <c r="B6" s="26" t="s">
         <v>533</v>
@@ -7608,7 +7615,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="24"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="25"/>
       <c r="B7" s="26" t="s">
         <v>534</v>
@@ -7623,7 +7630,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="23"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7632,7 +7639,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>511</v>
       </c>
@@ -7643,7 +7650,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="25"/>
       <c r="B10" s="26" t="s">
         <v>535</v>
@@ -7656,7 +7663,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="24"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="25"/>
       <c r="B11" s="26" t="s">
         <v>536</v>
@@ -7669,7 +7676,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="24"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="25"/>
       <c r="B12" s="26" t="s">
         <v>537</v>
@@ -7682,7 +7689,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="25"/>
       <c r="B13" s="26" t="s">
         <v>538</v>
@@ -7695,7 +7702,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="24"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="23"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7704,7 +7711,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="24"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>512</v>
       </c>
@@ -7715,7 +7722,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="24"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="25"/>
       <c r="B16" s="26" t="s">
         <v>540</v>
@@ -7730,7 +7737,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="25"/>
       <c r="B17" s="26" t="s">
         <v>543</v>
@@ -7743,7 +7750,7 @@
       <c r="F17" s="8"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="25"/>
       <c r="B18" s="26" t="s">
         <v>544</v>
@@ -7756,7 +7763,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="23"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7765,7 +7772,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>513</v>
       </c>
@@ -7776,7 +7783,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="25"/>
       <c r="B21" s="26" t="s">
         <v>545</v>
@@ -7789,7 +7796,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="25"/>
       <c r="B22" s="26" t="s">
         <v>546</v>
@@ -7802,7 +7809,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="25"/>
       <c r="B23" s="26" t="s">
         <v>547</v>
@@ -7815,7 +7822,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -7824,7 +7831,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -7833,7 +7840,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>514</v>
       </c>
@@ -7844,7 +7851,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="25"/>
       <c r="B27" s="26" t="s">
         <v>548</v>
@@ -7857,7 +7864,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="25"/>
       <c r="B28" s="26" t="s">
         <v>550</v>
@@ -7870,7 +7877,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="25"/>
       <c r="B29" s="26" t="s">
         <v>551</v>
@@ -7883,7 +7890,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -7892,7 +7899,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="24"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
         <v>553</v>
       </c>
@@ -7905,7 +7912,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="25"/>
       <c r="B32" s="26" t="s">
         <v>555</v>
@@ -7918,7 +7925,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="25"/>
       <c r="B33" s="26" t="s">
         <v>556</v>
@@ -7931,7 +7938,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="25"/>
       <c r="B34" s="26" t="s">
         <v>557</v>
@@ -7946,7 +7953,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="24"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="23"/>
       <c r="B35" s="26" t="s">
         <v>558</v>
@@ -7959,7 +7966,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="24"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="26" t="s">
         <v>559</v>
@@ -7972,7 +7979,7 @@
       <c r="F36" s="8"/>
       <c r="G36" s="24"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="25"/>
       <c r="B37" s="26" t="s">
         <v>561</v>
@@ -7985,7 +7992,7 @@
       <c r="F37" s="8"/>
       <c r="G37" s="24"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="23" t="s">
         <v>515</v>
       </c>
@@ -7996,7 +8003,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="25"/>
       <c r="B39" s="26" t="s">
         <v>562</v>
@@ -8009,7 +8016,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="24"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="25"/>
       <c r="B40" s="26" t="s">
         <v>563</v>
@@ -8022,7 +8029,7 @@
       <c r="F40" s="8"/>
       <c r="G40" s="24"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="25"/>
       <c r="B41" s="26" t="s">
         <v>564</v>
@@ -8035,7 +8042,7 @@
       <c r="F41" s="8"/>
       <c r="G41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="25"/>
       <c r="B42" s="26" t="s">
         <v>565</v>
@@ -8048,7 +8055,7 @@
       <c r="F42" s="8"/>
       <c r="G42" s="24"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="23"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -8057,7 +8064,7 @@
       <c r="F43" s="8"/>
       <c r="G43" s="24"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="23" t="s">
         <v>516</v>
       </c>
@@ -8068,7 +8075,7 @@
       <c r="F44" s="8"/>
       <c r="G44" s="24"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="25"/>
       <c r="B45" s="26" t="s">
         <v>566</v>
@@ -8081,7 +8088,7 @@
       <c r="F45" s="8"/>
       <c r="G45" s="24"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="25"/>
       <c r="B46" s="26" t="s">
         <v>567</v>
@@ -8094,7 +8101,7 @@
       <c r="F46" s="8"/>
       <c r="G46" s="24"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="25"/>
       <c r="B47" s="26" t="s">
         <v>568</v>
@@ -8107,7 +8114,7 @@
       <c r="F47" s="8"/>
       <c r="G47" s="24"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="25"/>
       <c r="B48" s="26" t="s">
         <v>569</v>
@@ -8120,7 +8127,7 @@
       <c r="F48" s="8"/>
       <c r="G48" s="24"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="23"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -8129,7 +8136,7 @@
       <c r="F49" s="8"/>
       <c r="G49" s="24"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="23" t="s">
         <v>517</v>
       </c>
@@ -8140,7 +8147,7 @@
       <c r="F50" s="8"/>
       <c r="G50" s="24"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="25"/>
       <c r="B51" s="26" t="s">
         <v>570</v>
@@ -8155,7 +8162,7 @@
       <c r="F51" s="8"/>
       <c r="G51" s="24"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="25"/>
       <c r="B52" s="26" t="s">
         <v>518</v>
@@ -8168,7 +8175,7 @@
       <c r="F52" s="8"/>
       <c r="G52" s="24"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="23"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -8177,7 +8184,7 @@
       <c r="F53" s="8"/>
       <c r="G53" s="24"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>519</v>
       </c>
@@ -8188,7 +8195,7 @@
       <c r="F54" s="8"/>
       <c r="G54" s="24"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="25"/>
       <c r="B55" s="26" t="s">
         <v>571</v>
@@ -8201,7 +8208,7 @@
       <c r="F55" s="8"/>
       <c r="G55" s="24"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="25"/>
       <c r="B56" s="26" t="s">
         <v>520</v>
@@ -8216,7 +8223,7 @@
       <c r="F56" s="8"/>
       <c r="G56" s="24"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="27"/>
       <c r="B57" s="28" t="s">
         <v>521</v>
@@ -8227,19 +8234,19 @@
       <c r="F57" s="29"/>
       <c r="G57" s="30"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B58" s="20"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B59" s="20"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="22"/>
     </row>
   </sheetData>
@@ -8253,20 +8260,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="I25" sqref="I24:I25"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="27.08203125" customWidth="1"/>
     <col min="2" max="2" width="9.75" customWidth="1"/>
-    <col min="3" max="3" width="60.375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
     <col min="4" max="4" width="70.75" customWidth="1"/>
-    <col min="5" max="5" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
         <v>580</v>
       </c>
@@ -8290,7 +8297,7 @@
       </c>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
       <c r="B3" s="26">
         <v>1</v>
@@ -8308,7 +8315,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>2</v>
       </c>
@@ -8322,7 +8329,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>585</v>
       </c>
@@ -8330,7 +8337,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>3</v>
       </c>
@@ -8344,7 +8351,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1</v>
       </c>
@@ -8358,7 +8365,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>2</v>
       </c>
@@ -8369,7 +8376,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>3</v>
       </c>
@@ -8383,7 +8390,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>1</v>
       </c>
@@ -8394,7 +8401,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>2</v>
       </c>
@@ -8405,7 +8412,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>3</v>
       </c>
@@ -8419,7 +8426,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>3</v>
       </c>
@@ -8430,7 +8437,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>1</v>
       </c>
@@ -8444,7 +8451,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>1</v>
       </c>
@@ -8455,7 +8462,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>2</v>
       </c>
@@ -8472,7 +8479,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="132" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="136" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>2</v>
       </c>
@@ -8486,7 +8493,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="34" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>2</v>
       </c>
@@ -8500,7 +8507,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>2</v>
       </c>
@@ -8514,7 +8521,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>1</v>
       </c>
@@ -8525,7 +8532,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="51" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>3</v>
       </c>
@@ -8539,7 +8546,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>1</v>
       </c>
@@ -8550,7 +8557,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="34" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>2</v>
       </c>
@@ -8564,21 +8571,21 @@
         <v>633</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="34" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>636</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>637</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>638</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="85" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>3</v>
       </c>
@@ -8586,7 +8593,10 @@
         <v>635</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>636</v>
+        <v>639</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add(p2493) O(n^2) 성능이라 시간초과
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="685">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3706,6 +3706,23 @@
 그렇다고 이걸 예외처리하자니 그것도 굉장히 로직이 지저분했다.
 문자열 파싱하지말고 숫자, 연산자 각자 배열에 넣는 방향으로 하자
 파싱해서 변경하면 너무 생각치 못한 에러가 생긴다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탑(p2493)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(n^2)을 O(n)으로 만들어야 풀리는 문제
+&gt;&gt; 스택을 이용하면 되는데,,,,,, 못찾았다ㅜ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>못품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스택</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8448,8 +8465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8993,7 +9010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -9034,9 +9051,7 @@
       <c r="A3" t="s">
         <v>673</v>
       </c>
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
+      <c r="B3" s="26"/>
       <c r="C3" s="8" t="s">
         <v>675</v>
       </c>
@@ -9050,8 +9065,19 @@
       <c r="G3" s="8"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E4" s="8"/>
+    <row r="4" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" s="8"/>

</xml_diff>

<commit_message>
complete(hacker rank - formatingMagicSquae)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -17,7 +17,7 @@
     <sheet name="프로그래머스 고득점" sheetId="3" r:id="rId3"/>
     <sheet name="프로그래머스 일일문제풀이" sheetId="4" r:id="rId4"/>
     <sheet name="백준 랜덤" sheetId="6" r:id="rId5"/>
-    <sheet name="해커랭크" sheetId="7" r:id="rId6"/>
+    <sheet name="hackerrank" sheetId="7" r:id="rId6"/>
     <sheet name="leetcode" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="808">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4270,6 +4270,21 @@
   </si>
   <si>
     <t>풀음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forming a Magic Square | HackerRank</t>
+  </si>
+  <si>
+    <t>정답인 행렬일 때 각 행,열,대각의 합이 15라는 것을 확인하고 이걸 체크해서 답을 구하려고 했다.
+확인하는 방향은 맞았지만 너무 구현이 오래걸리는 알고리즘이라 클렸다는 걸 직감했다.
+합이 15인 행,열,대각을 fixed로 고정시키고, 1개만 다른 경우만 15-(나머지)로 변경할 생각이었다. 정답인 배열을 리턴하는게 문제의 핵심이 아니엇기 때문에 할 필요 없었다..
+미리 답에 대한 결과를 세팅한 후 cost를 비교하는 방법이 최선이었다.
+답도 이렇게 해야 더 쉽고 빠르게 찾는다. 좋은 문제 풀이 접근 방향인 것 가탇.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>못품</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10274,8 +10289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10340,8 +10355,19 @@
         <v>804</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="8"/>
+    <row r="5" spans="1:8" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>775</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>805</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D6" s="4"/>
@@ -10571,9 +10597,10 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="https://www.hackerrank.com/challenges/simple-array-sum/"/>
+    <hyperlink ref="C5" r:id="rId2" display="https://www.hackerrank.com/challenges/magic-square-forming/problem?isFullScreen=true"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete(쿠팡 기출 - past1)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="백준 랜덤" sheetId="6" r:id="rId5"/>
     <sheet name="hackerrank" sheetId="7" r:id="rId6"/>
     <sheet name="leetcode" sheetId="9" r:id="rId7"/>
+    <sheet name="라이브 코딩 기출" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="837">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4351,6 +4352,104 @@
   </si>
   <si>
     <t>원래 구하려던 풀이로 풀었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//member.csv 파일 일부 
+이름, 취미, 소개 
+김프로, 축구:농구:야구, 구기종목 좋아요 
+정프로, 개발:당구:족구, 개발하는데 뛰긴 싫어 
+앙몬드, 피아노, 죠르디가 좋아요 좋아좋아너무좋아 
+죠르디, 스포츠댄스:개발, 개발하는 죠르디 
+…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취미별 인원수를 구하라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>public void printMemberCountGroupByHobby(){
+  List&lt;List&lt;String&gt;&gt; persons = CsvReader.getLines();
+  persons.remove(0);
+  Map&lt;String, Integer&gt; result = new HashMap&lt;&gt;();
+  //결과를 담을 해시맵 구성
+  persons.stream()
+    .flatMap(member-&gt;Arrays.stream(member.get(1).split(":")))
+    .forEach(hobby-&gt;result.merge(hobby, 1, (oldValue, newValue)-&gt;++oldValue));
+  //결과 출력
+  result.entrySet().forEach(entry-&gt;System.out.println(entry.getKey()+" "+entry.getValue()));
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취미별 정씨 성을 갖는 멤버 수를 구하라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>public void printMemberCountGroupByJeongMember(){
+  List&lt;List&lt;String&gt;&gt; lines = CsvReader.getLines();
+  lines.remove(0);
+  Map&lt;String, Integer&gt; result = new HashMap&lt;&gt;();
+  lines.stream()
+    .filter(member-&gt;member.get(0).startWith("정"))
+    .flatMap(member-&gt; Arrays.stream(member.get(1).split(":")))
+    .forEach(hobby-&gt;result.merge(hobby, 1, (oldValue, newValue)-&gt;++oldValue));
+  //출력
+  result.entrySet().forEach(entry-&gt;System.out.println(entry.getKey()+" "+entry.getValue()));
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소개 내용에 '좋아' 가 몇 번 등장하는지 구하라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>public void printLikeCount(){
+  List&lt;List&lt;String&gt;&gt; lines = CsvReader.getLines();
+  lines.remove(0);
+  final String word = "좋아";
+  int result = lines.stream()
+    .map(member -&gt; countfindString(member.get(2), word))
+    .reduce(0, Integer::sum);
+  //출력
+  System.out.println(word+" "+result);
+}
+private int countFindString(String source, String target){
+  int idx =source.indexOf(target);
+  if(idx==-1){
+    return 0;
+  }else{
+    return 1+countFindString(source.substring(idx+1), target);
+  }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 문제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Input: matrix = [[1,2,3],[4,5,6],[7,8,9]]
+Output: [1,2,3,6,9,8,7,4,5]
+Input: matrix = [[1,2,3,4],[5,6,7,8],[9,10,11,12]]
+Output: [1,2,3,4,8,12,11,10,9,5,6,7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출저 모름1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>past1.java
+잘 푼 풀이는 아닌것 같지만 그냥 풀었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠팡
+라이브 코딩
+기출</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4732,6 +4831,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1438276</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1380125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638301" y="10934701"/>
+          <a:ext cx="1352550" cy="1342024"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2028825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3342674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="12925425"/>
+          <a:ext cx="1743075" cy="1313849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -10751,7 +10931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -11066,4 +11246,347 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="60.375" customWidth="1"/>
+    <col min="4" max="4" width="91.375" customWidth="1"/>
+    <col min="5" max="5" width="25.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>577</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>522</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>571</v>
+      </c>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="26">
+        <v>2</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>825</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="26">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>828</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="8"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>833</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="22"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16" s="34"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="4"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="4"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="4"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="4"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="4"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="4"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="4"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="4"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="4"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="4"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="4"/>
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D35" s="4"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="4"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="4"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D38" s="4"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D41" s="4"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="22"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D53" s="4"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D55" s="4"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D57" s="4"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D59" s="4"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D60" s="4"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D61" s="4"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D62" s="4"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D63" s="4"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D64" s="4"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D65" s="4"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D68" s="4"/>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete(leetcd - ZigZag Conversion)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="842">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4510,6 +4510,17 @@
   </si>
   <si>
     <t>성능 통과 못함&gt;&gt; 다시풀기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zigzag Conversion - LeetCode</t>
+  </si>
+  <si>
+    <t>dx, dy 보다 rowString으로 해서 append하는게 쉬운 풀이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풀음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10992,7 +11003,7 @@
   <dimension ref="A2:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11086,7 +11097,18 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" s="10"/>
+      <c r="B7" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>839</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>840</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E8" s="10"/>
@@ -11311,9 +11333,10 @@
     <hyperlink ref="C4" r:id="rId1" display="https://leetcode.com/problems/two-sum/submissions/"/>
     <hyperlink ref="C5" r:id="rId2" display="https://leetcode.com/problems/longest-palindromic-substring/"/>
     <hyperlink ref="C6" r:id="rId3" display="https://leetcode.com/problems/3sum/submissions/"/>
+    <hyperlink ref="C7" r:id="rId4" display="https://leetcode.com/problems/zigzag-conversion/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete(leetcd - Reverse Integer)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="848">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4528,6 +4528,18 @@
   </si>
   <si>
     <t>for문을 r기준으로 loop를 돌아서 한 5분 버렸다.. 정신차리자..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풀음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse Integer - LeetCode</t>
+  </si>
+  <si>
+    <t>stringbuilder reverse를 잊고있었다. 
+이 문제는 exception 이용하는게 편한 문제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -10683,8 +10695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11025,8 +11037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11133,8 +11145,19 @@
         <v>841</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E8" s="10"/>
+    <row r="8" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>845</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>846</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" s="10"/>
@@ -11357,9 +11380,10 @@
     <hyperlink ref="C5" r:id="rId2" display="https://leetcode.com/problems/longest-palindromic-substring/"/>
     <hyperlink ref="C6" r:id="rId3" display="https://leetcode.com/problems/3sum/submissions/"/>
     <hyperlink ref="C7" r:id="rId4" display="https://leetcode.com/problems/zigzag-conversion/"/>
+    <hyperlink ref="C8" r:id="rId5" display="https://leetcode.com/problems/reverse-integer/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add(hkrk - Queens Attack2)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="850">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4544,6 +4544,13 @@
   </si>
   <si>
     <t>풀음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Queen's Attack II | HackerRank</t>
+  </si>
+  <si>
+    <t>엣지케이스 걸림</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11038,7 +11045,7 @@
   <dimension ref="A2:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11160,7 +11167,15 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E9" s="10"/>
+      <c r="B9" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>848</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E10" s="10"/>
@@ -11381,9 +11396,10 @@
     <hyperlink ref="C6" r:id="rId3" display="https://leetcode.com/problems/3sum/submissions/"/>
     <hyperlink ref="C7" r:id="rId4" display="https://leetcode.com/problems/zigzag-conversion/"/>
     <hyperlink ref="C8" r:id="rId5" display="https://leetcode.com/problems/reverse-integer/"/>
+    <hyperlink ref="C9" r:id="rId6" display="https://www.hackerrank.com/challenges/queens-attack-2/problem?isFullScreen=true"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete(hkrk - queen attack2)
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="851">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4551,6 +4551,11 @@
   </si>
   <si>
     <t>엣지케이스 걸림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원래 풀이가 왜 성능타임아웃과 엣지케이스가 있는지는 잘 모르겠다.
+callStack이 깊어져서 문제가 생긴걸까? 잘 모르겠다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11166,12 +11171,15 @@
         <v>847</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>848</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>850</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>849</v>

</xml_diff>

<commit_message>
chore : docs 정리
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="852">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4556,6 +4556,10 @@
   <si>
     <t>원래 풀이가 왜 성능타임아웃과 엣지케이스가 있는지는 잘 모르겠다.
 callStack이 깊어져서 문제가 생긴걸까? 잘 모르겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정렬 후 left right를 감소시켜가며 푸는게 효 성능통과 가능하다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11050,7 +11054,7 @@
   <dimension ref="A2:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11138,7 +11142,9 @@
       <c r="C6" s="22" t="s">
         <v>837</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>851</v>
+      </c>
       <c r="E6" s="10" t="s">
         <v>838</v>
       </c>

</xml_diff>

<commit_message>
add : docs 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="867">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4560,6 +4560,60 @@
   </si>
   <si>
     <t>정렬 후 left right를 감소시켜가며 푸는게 효 성능통과 가능하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shortest Subarray with Sum at Least K - LeetCode</t>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Duplicate Substring - LeetCode</t>
+  </si>
+  <si>
+    <t>study2_num2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study3_num1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subarray Sum Equals K - LeetCode</t>
+  </si>
+  <si>
+    <t>Restore IP Addresses - LeetCode</t>
+  </si>
+  <si>
+    <t>성능 걸림 &gt;&gt; 다시풀기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간 부족 &gt;&gt; 다시풀기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sliding Window Maximum - LeetCode</t>
+  </si>
+  <si>
+    <t>study3_num2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study3_num4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study3_num3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spiral Matrix - LeetCode</t>
+  </si>
+  <si>
+    <t>풀음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4771,7 +4825,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4878,6 +4932,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11051,15 +11108,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H68"/>
+  <dimension ref="A2:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="9.75" customWidth="1"/>
     <col min="3" max="3" width="60.375" customWidth="1"/>
     <col min="4" max="4" width="73.5" customWidth="1"/>
@@ -11195,141 +11252,205 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E11" s="10"/>
+      <c r="A11" t="s">
+        <v>855</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>853</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>852</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>859</v>
+      </c>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E12" s="10"/>
+      <c r="A12" t="s">
+        <v>856</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>853</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>854</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E13" s="10"/>
+      <c r="A13" t="s">
+        <v>862</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E14" s="10"/>
+      <c r="A14" t="s">
+        <v>864</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="34"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" t="s">
+        <v>863</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>853</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D16" s="4"/>
+      <c r="B16" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>857</v>
+      </c>
+      <c r="D16" s="34"/>
       <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="26"/>
+      <c r="C19" s="22"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="4"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="4"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="4"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D23" s="4"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D24" s="4"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D25" s="4"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D26" s="4"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D27" s="4"/>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D28" s="4"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D29" s="4"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D30" s="4"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D31" s="4"/>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D32" s="4"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33" s="4"/>
-      <c r="E33" s="11"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D34" s="4"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D35" s="4"/>
-      <c r="E35" s="11"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D36" s="4"/>
-      <c r="E36" s="10"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D37" s="4"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E38" s="10"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="11"/>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="11"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D40" s="4"/>
-      <c r="E40" s="10"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="11"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D42" s="22"/>
-      <c r="E42" s="10"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E43" s="11"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E44" s="10"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E45" s="11"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E46" s="10"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E47" s="11"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E48" s="10"/>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E49" s="10"/>
@@ -11341,28 +11462,27 @@
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D52" s="4"/>
       <c r="E52" s="10"/>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D53" s="4"/>
       <c r="E53" s="10"/>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D54" s="4"/>
       <c r="E54" s="10"/>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D55" s="4"/>
       <c r="E55" s="10"/>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D56" s="4"/>
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D57" s="4"/>
       <c r="E57" s="10"/>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D58" s="4"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.3">
@@ -11390,17 +11510,21 @@
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D65" s="4"/>
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D67" s="4"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D68" s="4"/>
       <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -11411,9 +11535,15 @@
     <hyperlink ref="C7" r:id="rId4" display="https://leetcode.com/problems/zigzag-conversion/"/>
     <hyperlink ref="C8" r:id="rId5" display="https://leetcode.com/problems/reverse-integer/"/>
     <hyperlink ref="C9" r:id="rId6" display="https://www.hackerrank.com/challenges/queens-attack-2/problem?isFullScreen=true"/>
+    <hyperlink ref="C11" r:id="rId7" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/"/>
+    <hyperlink ref="C12" r:id="rId8" display="https://leetcode.com/problems/longest-duplicate-substring/"/>
+    <hyperlink ref="C16" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C13" r:id="rId10" display="https://leetcode.com/problems/restore-ip-addresses/"/>
+    <hyperlink ref="C15" r:id="rId11" display="https://leetcode.com/problems/sliding-window-maximum/"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/spiral-matrix/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
complete(study2-num1): 정리 및 솔루션 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="874">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4627,6 +4627,23 @@
   <si>
     <t>Monotone Queue Optimization 문제
 배열 사이즈를 1 증가시킴으로써 누적합 배열을 깔끔하게 만들 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Two Sum - LeetCode</t>
+  </si>
+  <si>
+    <t>study2_num1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leetcode 솔루션을 보니, 다양한 Approach가 존재한다는 것을 알았다.
+HashMap을 사용해서 하는 풀이가 내가 풀었던 것보다 시간복잡도가 줄어든다.
+내 풀이는 공간복잡도가 O(1)이지만 시간복잡도는 O(NlongN)이므로 이런 것을 확실히 알아야 할 필요가 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔루션 정리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11124,7 +11141,7 @@
   <dimension ref="A2:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11178,7 +11195,7 @@
       <c r="H3" s="24"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="26" t="s">
         <v>798</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -11261,8 +11278,22 @@
         <v>849</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E10" s="10"/>
+    <row r="10" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>871</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>798</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>870</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -11566,9 +11597,10 @@
     <hyperlink ref="C15" r:id="rId11" display="https://leetcode.com/problems/sliding-window-maximum/"/>
     <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/spiral-matrix/"/>
     <hyperlink ref="C12" r:id="rId13" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/solution/"/>
+    <hyperlink ref="C10" r:id="rId14" display="https://leetcode.com/problems/two-sum/solution/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add : RestoreIpAddress 초안
- 오랜만에 풀어서 공간복잡도가 복잡하게 풀었다.
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="9975" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BASIC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="892">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4670,49 +4670,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>study3.num3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study3.num2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study3.num1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study2.num2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study2.num1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간단한 팰린드롬도 이렇게 O(N) -&gt; O(log10(N)으로 단축 가능하다는거에 놀람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shortest_Subarray_with_Sum_at_Least_K</t>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/</t>
+  </si>
+  <si>
+    <t>하드답게 너무 어렵다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이해완료 &gt;&gt; 다시풀기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>study3.num4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>study3.num3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study3.num2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study3.num1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study2.num2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>study2.num1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>간단한 팰린드롬도 이렇게 O(N) -&gt; O(log10(N)으로 단축 가능하다는거에 놀람</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shortest_Subarray_with_Sum_at_Least_K</t>
-  </si>
-  <si>
-    <t>Hard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/</t>
-  </si>
-  <si>
-    <t>하드답게 너무 어렵다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이해완료 &gt;&gt; 다시풀기</t>
+    <t>DFS로 풀었다. 너무 정리가 안되도록 풀었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RestoreIpAddress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간복잡도 낭비가 너무 심하게 풀었다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11358,8 +11370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11498,7 +11510,7 @@
     </row>
     <row r="10" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>798</v>
@@ -11515,7 +11527,7 @@
     </row>
     <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>852</v>
@@ -11533,7 +11545,7 @@
     </row>
     <row r="12" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>774</v>
@@ -11550,7 +11562,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>774</v>
@@ -11558,13 +11570,16 @@
       <c r="C13" s="22" t="s">
         <v>855</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>889</v>
+      </c>
       <c r="E13" s="10" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>774</v>
@@ -11578,7 +11593,7 @@
     </row>
     <row r="15" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>877</v>
+        <v>888</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>852</v>
@@ -11625,28 +11640,40 @@
         <v>873</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>883</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>884</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" t="s">
         <v>885</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>886</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="10" t="s">
         <v>887</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>888</v>
-      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>890</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>855</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>891</v>
+      </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -11654,6 +11681,9 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -11844,9 +11874,10 @@
     <hyperlink ref="C12" r:id="rId13" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/solution/"/>
     <hyperlink ref="C10" r:id="rId14" display="https://leetcode.com/problems/two-sum/solution/"/>
     <hyperlink ref="C18" r:id="rId15"/>
+    <hyperlink ref="C20" r:id="rId16" display="https://leetcode.com/problems/restore-ip-addresses/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -11854,7 +11885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -12197,7 +12228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add : RestoreIpAddress 2안
- dfs에서 재귀 호출후 원복하는 로직으로 추가 구현
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -4704,10 +4704,6 @@
     <t>https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/</t>
   </si>
   <si>
-    <t>하드답게 너무 어렵다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이해완료 &gt;&gt; 다시풀기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4724,7 +4720,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공간복잡도 낭비가 너무 심하게 풀었다.</t>
+    <t>공간복잡도 낭비가 너무 심하게 풀었다.
+list대신 depth와 StringBuilder를 넘겨준다면 더욱 효율적으로 풀 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간복잡도 낭비가 너무 심하게 풀었다.
+list대신 depth와 StringBuilder를 넘겨준다면 더욱 효율적으로 풀 수 있다.
+DFS에서 공간속잡도를 줄이기 위해서 재귀를 탄 후 
+append 했던 부분을 제거해줘야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11370,8 +11374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11571,7 +11575,7 @@
         <v>855</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>857</v>
@@ -11593,7 +11597,7 @@
     </row>
     <row r="15" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>852</v>
@@ -11644,7 +11648,7 @@
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>883</v>
       </c>
@@ -11654,16 +11658,16 @@
       <c r="C19" t="s">
         <v>885</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>886</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>774</v>

</xml_diff>

<commit_message>
add : SubArraySumEqualK - 성능 미통과
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="894">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4571,9 +4571,6 @@
     <t>Longest Duplicate Substring - LeetCode</t>
   </si>
   <si>
-    <t>Subarray Sum Equals K - LeetCode</t>
-  </si>
-  <si>
     <t>Restore IP Addresses - LeetCode</t>
   </si>
   <si>
@@ -4729,6 +4726,19 @@
   <si>
     <t>하드답게 너무 어렵다.
 누적합으로 만들고 새로운 문제풀이 접근방식으로 풀어야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subarray Sum Equals K - LeetCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubArraySumEqualK</t>
+  </si>
+  <si>
+    <t>dfs로 구현 
+3항 연산자 이슈, return 위치때문에 dfs가 0-n까지 안도는 이슈
+-&gt;성능 못통과</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11374,13 +11384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="29.25" customWidth="1"/>
     <col min="2" max="2" width="9.75" customWidth="1"/>
     <col min="3" max="3" width="60.375" customWidth="1"/>
     <col min="4" max="4" width="73.5" customWidth="1"/>
@@ -11389,7 +11399,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>780</v>
@@ -11514,102 +11524,102 @@
     </row>
     <row r="10" spans="1:8" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>798</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>864</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>865</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="10" t="s">
         <v>866</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>852</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C12" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>862</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>863</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>859</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>852</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -11617,7 +11627,7 @@
         <v>774</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>854</v>
+        <v>891</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="10"/>
@@ -11635,59 +11645,67 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>881</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>882</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" t="s">
         <v>883</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>884</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>891</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="4"/>
+    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>892</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>891</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>893</v>
+      </c>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D22">
-        <v>1</v>
-      </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -11879,9 +11897,10 @@
     <hyperlink ref="C10" r:id="rId14" display="https://leetcode.com/problems/two-sum/solution/"/>
     <hyperlink ref="C18" r:id="rId15"/>
     <hyperlink ref="C20" r:id="rId16" display="https://leetcode.com/problems/restore-ip-addresses/"/>
+    <hyperlink ref="C21" r:id="rId17" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -12271,13 +12290,13 @@
     </row>
     <row r="2" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B2" s="26">
         <v>1</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="8"/>
@@ -12287,7 +12306,7 @@
     </row>
     <row r="3" spans="1:8" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12309,7 +12328,7 @@
     </row>
     <row r="6" spans="1:8" ht="378" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B6">
         <v>3</v>

</xml_diff>

<commit_message>
add : SubArraySumEqualK - 솔루션 추가
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="896">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4738,7 +4738,16 @@
   <si>
     <t>dfs로 구현 
 3항 연산자 이슈, return 위치때문에 dfs가 0-n까지 안도는 이슈
--&gt;성능 못통과</t>
+-&gt;성능 못통과
+누적합으로 만들어서 새로운 문제풀이 접근방식으로 풀어야한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubArraySumEqualK_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔루션 정리했다. 댜양한 방법으로 순서대로 정리되어 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11384,8 +11393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11690,7 +11699,7 @@
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>892</v>
       </c>
@@ -11706,6 +11715,18 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>894</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>891</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>895</v>
+      </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -11898,9 +11919,10 @@
     <hyperlink ref="C18" r:id="rId15"/>
     <hyperlink ref="C20" r:id="rId16" display="https://leetcode.com/problems/restore-ip-addresses/"/>
     <hyperlink ref="C21" r:id="rId17" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C22" r:id="rId18" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add : LongestDuplicateSubstring 시작
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="896">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4694,9 +4694,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/</t>
-  </si>
-  <si>
     <t>이해완료 &gt;&gt; 다시풀기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4749,6 +4746,9 @@
   <si>
     <t>솔루션 정리했다. 댜양한 방법으로 순서대로 정리되어 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LongestDuplicateSubstring</t>
   </si>
 </sst>
 </file>
@@ -4959,7 +4959,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5070,6 +5070,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11393,8 +11408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11549,19 +11564,19 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="37" t="s">
         <v>879</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>852</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="39" t="s">
         <v>860</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="40" t="s">
         <v>863</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="41" t="s">
         <v>855</v>
       </c>
       <c r="F11" s="10"/>
@@ -11584,19 +11599,19 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="37" t="s">
         <v>877</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="38" t="s">
         <v>774</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="39" t="s">
         <v>854</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>886</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="40" t="s">
+        <v>885</v>
+      </c>
+      <c r="E13" s="41" t="s">
         <v>856</v>
       </c>
     </row>
@@ -11616,7 +11631,7 @@
     </row>
     <row r="15" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>852</v>
@@ -11636,13 +11651,16 @@
         <v>774</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>895</v>
+      </c>
       <c r="B17" s="36" t="s">
         <v>852</v>
       </c>
@@ -11663,7 +11681,7 @@
         <v>872</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E18" s="10"/>
     </row>
@@ -11674,19 +11692,19 @@
       <c r="B19" s="26" t="s">
         <v>882</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>889</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>883</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>890</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>774</v>
@@ -11695,37 +11713,37 @@
         <v>854</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>774</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E22" s="10"/>
     </row>
@@ -11920,9 +11938,10 @@
     <hyperlink ref="C20" r:id="rId16" display="https://leetcode.com/problems/restore-ip-addresses/"/>
     <hyperlink ref="C21" r:id="rId17" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
     <hyperlink ref="C22" r:id="rId18" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C19" r:id="rId19" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add : LongestDuplicateSubstring 푸는중
</commit_message>
<xml_diff>
--- a/doc/알고리즘 문제 목록.xlsx
+++ b/doc/알고리즘 문제 목록.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="897">
   <si>
     <t>수학</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4749,6 +4749,10 @@
   </si>
   <si>
     <t>LongestDuplicateSubstring</t>
+  </si>
+  <si>
+    <t>브루트 포스 O(n^3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -11408,8 +11412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11647,29 +11651,12 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
-        <v>774</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>890</v>
-      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="34"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>895</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>852</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>853</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="10"/>
-    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>875</v>
@@ -11748,14 +11735,37 @@
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D23" s="4"/>
+      <c r="A23" t="s">
+        <v>895</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>852</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>853</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>896</v>
+      </c>
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
+        <v>774</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>890</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="36" t="s">
+        <v>852</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>857</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="11"/>
     </row>
@@ -11927,21 +11937,22 @@
     <hyperlink ref="C8" r:id="rId5" display="https://leetcode.com/problems/reverse-integer/"/>
     <hyperlink ref="C9" r:id="rId6" display="https://www.hackerrank.com/challenges/queens-attack-2/problem?isFullScreen=true"/>
     <hyperlink ref="C11" r:id="rId7" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/"/>
-    <hyperlink ref="C17" r:id="rId8" display="https://leetcode.com/problems/longest-duplicate-substring/"/>
-    <hyperlink ref="C16" r:id="rId9" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
-    <hyperlink ref="C13" r:id="rId10" display="https://leetcode.com/problems/restore-ip-addresses/"/>
-    <hyperlink ref="C15" r:id="rId11" display="https://leetcode.com/problems/sliding-window-maximum/"/>
-    <hyperlink ref="C14" r:id="rId12" display="https://leetcode.com/problems/spiral-matrix/"/>
-    <hyperlink ref="C12" r:id="rId13" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/solution/"/>
-    <hyperlink ref="C10" r:id="rId14" display="https://leetcode.com/problems/two-sum/solution/"/>
-    <hyperlink ref="C18" r:id="rId15"/>
-    <hyperlink ref="C20" r:id="rId16" display="https://leetcode.com/problems/restore-ip-addresses/"/>
-    <hyperlink ref="C21" r:id="rId17" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
-    <hyperlink ref="C22" r:id="rId18" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
-    <hyperlink ref="C19" r:id="rId19" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/"/>
+    <hyperlink ref="C23" r:id="rId8" display="https://leetcode.com/problems/longest-duplicate-substring/"/>
+    <hyperlink ref="C13" r:id="rId9" display="https://leetcode.com/problems/restore-ip-addresses/"/>
+    <hyperlink ref="C15" r:id="rId10" display="https://leetcode.com/problems/sliding-window-maximum/"/>
+    <hyperlink ref="C14" r:id="rId11" display="https://leetcode.com/problems/spiral-matrix/"/>
+    <hyperlink ref="C12" r:id="rId12" display="https://leetcode.com/problems/longest-substring-without-repeating-characters/solution/"/>
+    <hyperlink ref="C10" r:id="rId13" display="https://leetcode.com/problems/two-sum/solution/"/>
+    <hyperlink ref="C18" r:id="rId14"/>
+    <hyperlink ref="C20" r:id="rId15" display="https://leetcode.com/problems/restore-ip-addresses/"/>
+    <hyperlink ref="C21" r:id="rId16" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C22" r:id="rId17" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C19" r:id="rId18" display="https://leetcode.com/problems/shortest-subarray-with-sum-at-least-k/"/>
+    <hyperlink ref="C24" r:id="rId19" display="https://leetcode.com/problems/subarray-sum-equals-k/"/>
+    <hyperlink ref="C25" r:id="rId20" display="https://leetcode.com/problems/sliding-window-maximum/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>